<commit_message>
direct and reverse final updated
</commit_message>
<xml_diff>
--- a/Phase_distribution_0.xlsx
+++ b/Phase_distribution_0.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B78"/>
+  <dimension ref="A1:B382"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,618 +440,3050 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>-526.3664371564615</v>
+        <v>-526.3472030509745</v>
       </c>
       <c r="B2" t="n">
-        <v>-219.042259250994</v>
+        <v>-30.54403340524266</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>-516.8404703177098</v>
+        <v>-524.4736779913088</v>
       </c>
       <c r="B3" t="n">
-        <v>-217.7501865067466</v>
+        <v>-30.28558534772463</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>-507.0348765551696</v>
+        <v>-522.5872033986449</v>
       </c>
       <c r="B4" t="n">
-        <v>-216.4739614483718</v>
+        <v>-30.02755566708299</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>-496.8879581541865</v>
+        <v>-520.6876946775437</v>
       </c>
       <c r="B5" t="n">
-        <v>-215.2051527351188</v>
+        <v>-29.76992492741658</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>-486.3974027371788</v>
+        <v>-518.7750457116435</v>
       </c>
       <c r="B6" t="n">
-        <v>-213.9440495020899</v>
+        <v>-29.51267254726389</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>-475.6110547879447</v>
+        <v>-516.8492212102877</v>
       </c>
       <c r="B7" t="n">
-        <v>-212.6969944921547</v>
+        <v>-29.25578906989051</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>-464.502475700235</v>
+        <v>-514.9101674327534</v>
       </c>
       <c r="B8" t="n">
-        <v>-211.4616364411701</v>
+        <v>-28.99926390209771</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>-453.067075405702</v>
+        <v>-512.9578688082988</v>
       </c>
       <c r="B9" t="n">
-        <v>-210.2385865648926</v>
+        <v>-28.74309272472178</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>-441.3788665601374</v>
+        <v>-510.9923110681352</v>
       </c>
       <c r="B10" t="n">
-        <v>-209.0366181576561</v>
+        <v>-28.48727242656781</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>-429.4271380935809</v>
+        <v>-509.0135058453289</v>
       </c>
       <c r="B11" t="n">
-        <v>-207.8552526380109</v>
+        <v>-28.23180419089238</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>-417.1468863202239</v>
+        <v>-507.021482121423</v>
       </c>
       <c r="B12" t="n">
-        <v>-206.6892714162506</v>
+        <v>-27.97669220664864</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>-404.6595039630812</v>
+        <v>-505.0162505185625</v>
       </c>
       <c r="B13" t="n">
-        <v>-205.5512000179198</v>
+        <v>-27.72193900510649</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>-391.8800802199513</v>
+        <v>-502.9978363153704</v>
       </c>
       <c r="B14" t="n">
-        <v>-204.4341833275083</v>
+        <v>-27.46754964961067</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>-378.9008137662296</v>
+        <v>-500.9663083704347</v>
       </c>
       <c r="B15" t="n">
-        <v>-203.3472295038764</v>
+        <v>-27.21353521949166</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>-365.6493457779485</v>
+        <v>-498.9216803158042</v>
       </c>
       <c r="B16" t="n">
-        <v>-202.2851977938585</v>
+        <v>-26.95990034360466</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>-352.1728874897445</v>
+        <v>-496.8640342401368</v>
       </c>
       <c r="B17" t="n">
-        <v>-201.2530109600901</v>
+        <v>-26.70665860204483</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>-338.5035579061357</v>
+        <v>-494.7934062370233</v>
       </c>
       <c r="B18" t="n">
-        <v>-200.2539189768253</v>
+        <v>-26.45381823716292</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>-324.6120722466455</v>
+        <v>-492.7098485792596</v>
       </c>
       <c r="B19" t="n">
-        <v>-199.2866268979265</v>
+        <v>-26.20138985102597</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>-310.4389547863594</v>
+        <v>-490.6134470420977</v>
       </c>
       <c r="B20" t="n">
-        <v>-198.3483619130257</v>
+        <v>-25.94938837611346</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>-296.1888668471196</v>
+        <v>-488.5042357404968</v>
       </c>
       <c r="B21" t="n">
-        <v>-197.4533649082997</v>
+        <v>-25.69782277363902</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>-281.726801504082</v>
+        <v>-486.3822983315987</v>
       </c>
       <c r="B22" t="n">
-        <v>-196.593551721649</v>
+        <v>-25.44670818551924</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>-267.0474869751354</v>
+        <v>-484.2477089985559</v>
       </c>
       <c r="B23" t="n">
-        <v>-195.7697731118441</v>
+        <v>-25.19605878016785</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>-252.2560592356868</v>
+        <v>-482.1005046069063</v>
       </c>
       <c r="B24" t="n">
-        <v>-194.9886551004076</v>
+        <v>-24.94588454647533</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>-237.2404891900013</v>
+        <v>-479.940791521815</v>
       </c>
       <c r="B25" t="n">
-        <v>-194.245087376088</v>
+        <v>-24.69620374919211</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>-222.0830049014547</v>
+        <v>-477.7686217431812</v>
       </c>
       <c r="B26" t="n">
-        <v>-193.5441564992296</v>
+        <v>-24.44702844352523</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>-206.8166896557542</v>
+        <v>-475.5840738250679</v>
       </c>
       <c r="B27" t="n">
-        <v>-192.8878899068154</v>
+        <v>-24.19837388157708</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>-191.3729577515274</v>
+        <v>-473.3872141442815</v>
       </c>
       <c r="B28" t="n">
-        <v>-192.2740608227566</v>
+        <v>-23.95025402236999</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>-175.8987039037172</v>
+        <v>-471.1781124276358</v>
       </c>
       <c r="B29" t="n">
-        <v>-191.7089053394388</v>
+        <v>-23.70268330666292</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>-160.1963559560739</v>
+        <v>-468.9568674908161</v>
       </c>
       <c r="B30" t="n">
-        <v>-191.1858934505467</v>
+        <v>-23.45567948327266</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>-144.4712268244831</v>
+        <v>-466.7235242997001</v>
       </c>
       <c r="B31" t="n">
-        <v>-190.7125692230233</v>
+        <v>-23.20925435443723</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>-128.6381867344297</v>
+        <v>-464.4781562687113</v>
       </c>
       <c r="B32" t="n">
-        <v>-190.2865415963255</v>
+        <v>-22.96342297528892</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>-112.750846950619</v>
+        <v>-462.2208691430645</v>
       </c>
       <c r="B33" t="n">
-        <v>-189.9096276404733</v>
+        <v>-22.71820394289267</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>-96.8193278643446</v>
+        <v>-459.9517071643301</v>
       </c>
       <c r="B34" t="n">
-        <v>-189.5821869758387</v>
+        <v>-22.47360917376716</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>-80.68086436404928</v>
+        <v>-457.6707503370602</v>
       </c>
       <c r="B35" t="n">
-        <v>-189.3017561463344</v>
+        <v>-22.22965451983504</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>-64.43877310544451</v>
+        <v>-455.3780719573454</v>
       </c>
       <c r="B36" t="n">
-        <v>-189.071367883151</v>
+        <v>-21.98635512064564</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>-48.3260376227026</v>
+        <v>-453.0737604705545</v>
       </c>
       <c r="B37" t="n">
-        <v>-188.8939815585254</v>
+        <v>-21.74372771718336</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>-32.37726035826057</v>
+        <v>-450.7578668088418</v>
       </c>
       <c r="B38" t="n">
-        <v>-188.7684433785307</v>
+        <v>-21.50178510173038</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>-15.82189508272829</v>
+        <v>-448.4304887754113</v>
       </c>
       <c r="B39" t="n">
-        <v>-188.6906588144519</v>
+        <v>-21.26054498021159</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>0.1257339890882191</v>
+        <v>-446.0916757036269</v>
       </c>
       <c r="B40" t="n">
-        <v>-188.6662564772984</v>
+        <v>-21.02002000651123</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>16.8460364552246</v>
+        <v>-443.7415254156298</v>
       </c>
       <c r="B41" t="n">
-        <v>-188.6939652255139</v>
+        <v>-20.78022783018451</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>32.74300940707079</v>
+        <v>-441.3800931065904</v>
       </c>
       <c r="B42" t="n">
-        <v>-188.7707616546505</v>
+        <v>-20.54118170617224</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>48.76978712043124</v>
+        <v>-439.0074496330629</v>
       </c>
       <c r="B43" t="n">
-        <v>-188.898184900581</v>
+        <v>-20.30289649384298</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>64.80811374152674</v>
+        <v>-436.6236817881099</v>
       </c>
       <c r="B44" t="n">
-        <v>-189.076033728793</v>
+        <v>-20.06538861661326</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>81.0920625804379</v>
+        <v>-434.2288536155687</v>
       </c>
       <c r="B45" t="n">
-        <v>-189.3082629470126</v>
+        <v>-19.82867218512735</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>97.04222184139724</v>
+        <v>-431.8230288394137</v>
       </c>
       <c r="B46" t="n">
-        <v>-189.5864178427028</v>
+        <v>-19.59276127469559</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>113.0874164372362</v>
+        <v>-429.4063016769393</v>
       </c>
       <c r="B47" t="n">
-        <v>-189.9170888533401</v>
+        <v>-19.35767290822088</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>129.0032254917002</v>
+        <v>-426.9787196594624</v>
       </c>
       <c r="B48" t="n">
-        <v>-190.2957957397257</v>
+        <v>-19.12341951450946</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>144.8106245461567</v>
+        <v>-424.5403765964429</v>
       </c>
       <c r="B49" t="n">
-        <v>-190.72225582089</v>
+        <v>-18.89001797146497</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>160.5582833694337</v>
+        <v>-422.0913193645184</v>
       </c>
       <c r="B50" t="n">
-        <v>-191.1973803614609</v>
+        <v>-18.65748060691388</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>176.1980636184321</v>
+        <v>-419.6316430757205</v>
       </c>
       <c r="B51" t="n">
-        <v>-191.7193680402188</v>
+        <v>-18.42582430538087</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>191.6935319941059</v>
+        <v>-417.161401175011</v>
       </c>
       <c r="B52" t="n">
-        <v>-192.2862964289998</v>
+        <v>-18.19506195396451</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>207.1546398832043</v>
+        <v>-414.6806595029104</v>
       </c>
       <c r="B53" t="n">
-        <v>-192.9018824093748</v>
+        <v>-17.96520758881886</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>222.4362494267129</v>
+        <v>-412.1895111671856</v>
       </c>
       <c r="B54" t="n">
-        <v>-193.5599291837401</v>
+        <v>-17.73627770674813</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>237.5460835424495</v>
+        <v>-409.6880034927844</v>
       </c>
       <c r="B55" t="n">
-        <v>-194.2597291221022</v>
+        <v>-17.50828452723346</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>252.5191299952177</v>
+        <v>-407.1762211723109</v>
       </c>
       <c r="B56" t="n">
-        <v>-195.0021219566485</v>
+        <v>-17.28124364980434</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>267.3524039271226</v>
+        <v>-404.6542299230811</v>
       </c>
       <c r="B57" t="n">
-        <v>-195.7863889614922</v>
+        <v>-17.05516888057554</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>281.9927167216334</v>
+        <v>-402.1220960579145</v>
       </c>
       <c r="B58" t="n">
-        <v>-196.608925608086</v>
+        <v>-16.83007403396198</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>296.4671809272901</v>
+        <v>-399.5798876257906</v>
       </c>
       <c r="B59" t="n">
-        <v>-197.4703874206668</v>
+        <v>-16.60597302877568</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>310.751188383268</v>
+        <v>-397.0276689807418</v>
       </c>
       <c r="B60" t="n">
-        <v>-198.3685118507364</v>
+        <v>-16.38287940674704</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>324.8778476224666</v>
+        <v>-394.4655298508153</v>
       </c>
       <c r="B61" t="n">
-        <v>-199.3046855891174</v>
+        <v>-16.16080885423938</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>338.7790506118218</v>
+        <v>-391.8935101358704</v>
       </c>
       <c r="B62" t="n">
-        <v>-200.2735866122136</v>
+        <v>-15.93977266969756</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>352.4363962043605</v>
+        <v>-389.3117038791105</v>
       </c>
       <c r="B63" t="n">
-        <v>-201.2727401478723</v>
+        <v>-15.71978676889586</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>365.8916551488791</v>
+        <v>-386.7201601537267</v>
       </c>
       <c r="B64" t="n">
-        <v>-202.3041942973318</v>
+        <v>-15.50086314596476</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>379.1511609631729</v>
+        <v>-384.1189631884458</v>
       </c>
       <c r="B65" t="n">
-        <v>-203.3677517330274</v>
+        <v>-15.28301671919758</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>392.1284198127567</v>
+        <v>-381.5081678648841</v>
       </c>
       <c r="B66" t="n">
-        <v>-204.4554426453352</v>
+        <v>-15.06625986872137</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>404.8965937484522</v>
+        <v>-378.8878458070191</v>
       </c>
       <c r="B67" t="n">
-        <v>-205.5723728977436</v>
+        <v>-14.85060631863783</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>417.381588848094</v>
+        <v>-376.2580717304365</v>
       </c>
       <c r="B68" t="n">
-        <v>-206.711115153801</v>
+        <v>-14.63606996653718</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>429.6342997416107</v>
+        <v>-373.6189085357614</v>
       </c>
       <c r="B69" t="n">
-        <v>-207.8753309708301</v>
+        <v>-14.42266367090804</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>441.5672510538319</v>
+        <v>-370.9704213535983</v>
       </c>
       <c r="B70" t="n">
-        <v>-209.0556197181159</v>
+        <v>-14.21040041303903</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>453.2927860062666</v>
+        <v>-368.3126813382383</v>
       </c>
       <c r="B71" t="n">
-        <v>-210.262267682533</v>
+        <v>-13.99929358788981</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>464.670888723478</v>
+        <v>-365.6457532115324</v>
       </c>
       <c r="B72" t="n">
-        <v>-211.4800092986483</v>
+        <v>-13.7893560057143</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>475.7453778183342</v>
+        <v>-362.9697110567643</v>
       </c>
       <c r="B73" t="n">
-        <v>-212.7122293570337</v>
+        <v>-13.58060114012082</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>486.5743198011792</v>
+        <v>-360.2846101496158</v>
       </c>
       <c r="B74" t="n">
-        <v>-213.9649116797992</v>
+        <v>-13.37304092591475</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>497.0240651841008</v>
+        <v>-357.5905270863293</v>
       </c>
       <c r="B75" t="n">
-        <v>-215.2218431007122</v>
+        <v>-13.16668888523517</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>507.1672271228913</v>
+        <v>-354.8875377911669</v>
       </c>
       <c r="B76" t="n">
-        <v>-216.4908485547319</v>
+        <v>-12.96155838946498</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>517.0054516873213</v>
+        <v>-352.1756880406816</v>
       </c>
       <c r="B77" t="n">
-        <v>-217.7721093682163</v>
+        <v>-12.75766045432735</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>526.4786631192428</v>
+        <v>-349.4550662725026</v>
       </c>
       <c r="B78" t="n">
-        <v>-219.0578115923426</v>
+        <v>-12.55500924409407</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>-346.725729889902</v>
+      </c>
+      <c r="B79" t="n">
+        <v>-12.35361650819092</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>-343.9877423655303</v>
+      </c>
+      <c r="B80" t="n">
+        <v>-12.15349438808275</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>-341.2411760537325</v>
+      </c>
+      <c r="B81" t="n">
+        <v>-11.95465559849347</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>-338.4861093025168</v>
+      </c>
+      <c r="B82" t="n">
+        <v>-11.75711318950343</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>-335.7225934097989</v>
+      </c>
+      <c r="B83" t="n">
+        <v>-11.56087818966265</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>-332.950703223969</v>
+      </c>
+      <c r="B84" t="n">
+        <v>-11.36596324032399</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>-330.170504973489</v>
+      </c>
+      <c r="B85" t="n">
+        <v>-11.17238028448674</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>-327.3820615317619</v>
+      </c>
+      <c r="B86" t="n">
+        <v>-10.98014095700756</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>-324.5854531104702</v>
+      </c>
+      <c r="B87" t="n">
+        <v>-10.78925800142039</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>-321.780737219365</v>
+      </c>
+      <c r="B88" t="n">
+        <v>-10.59974251707084</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>-318.9679906373345</v>
+      </c>
+      <c r="B89" t="n">
+        <v>-10.41160683053093</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>-316.1472731556824</v>
+      </c>
+      <c r="B90" t="n">
+        <v>-10.22486203997514</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>-313.3186566756283</v>
+      </c>
+      <c r="B91" t="n">
+        <v>-10.0395199707645</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>-310.4822121613699</v>
+      </c>
+      <c r="B92" t="n">
+        <v>-9.855592290958981</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>-307.6379993002128</v>
+      </c>
+      <c r="B93" t="n">
+        <v>-9.673089854520896</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>-304.7861010814561</v>
+      </c>
+      <c r="B94" t="n">
+        <v>-9.492024923259976</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>-301.9265710980048</v>
+      </c>
+      <c r="B95" t="n">
+        <v>-9.312407794329317</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>-299.0594918350333</v>
+      </c>
+      <c r="B96" t="n">
+        <v>-9.134250502397549</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>-296.18491773498</v>
+      </c>
+      <c r="B97" t="n">
+        <v>-8.957563240602951</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>-293.302925216938</v>
+      </c>
+      <c r="B98" t="n">
+        <v>-8.782357479434296</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>-290.413591503346</v>
+      </c>
+      <c r="B99" t="n">
+        <v>-8.608644626332449</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>-287.5169757972651</v>
+      </c>
+      <c r="B100" t="n">
+        <v>-8.436434909478038</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>-284.613160473918</v>
+      </c>
+      <c r="B101" t="n">
+        <v>-8.265739846422235</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>-281.7021884744555</v>
+      </c>
+      <c r="B102" t="n">
+        <v>-8.096568547260944</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>-278.7841477730352</v>
+      </c>
+      <c r="B103" t="n">
+        <v>-7.928932672446024</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>-275.8591151749225</v>
+      </c>
+      <c r="B104" t="n">
+        <v>-7.76284310823965</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>-272.9271508138009</v>
+      </c>
+      <c r="B105" t="n">
+        <v>-7.598309696786629</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>-269.9883366858234</v>
+      </c>
+      <c r="B106" t="n">
+        <v>-7.435343416108452</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>-267.0427211132242</v>
+      </c>
+      <c r="B107" t="n">
+        <v>-7.273953281731536</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>-264.0904039784929</v>
+      </c>
+      <c r="B108" t="n">
+        <v>-7.114151045131933</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>-261.1314281578338</v>
+      </c>
+      <c r="B109" t="n">
+        <v>-6.95594525161647</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>-258.1658813246446</v>
+      </c>
+      <c r="B110" t="n">
+        <v>-6.799346773285606</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>-255.1938357065515</v>
+      </c>
+      <c r="B111" t="n">
+        <v>-6.644365537449232</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="n">
+        <v>-252.2153450847416</v>
+      </c>
+      <c r="B112" t="n">
+        <v>-6.491010424700448</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="n">
+        <v>-249.2304976230438</v>
+      </c>
+      <c r="B113" t="n">
+        <v>-6.339291997572758</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="n">
+        <v>-246.2393763400055</v>
+      </c>
+      <c r="B114" t="n">
+        <v>-6.18922041657197</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="n">
+        <v>-243.2420245654639</v>
+      </c>
+      <c r="B115" t="n">
+        <v>-6.040803757598326</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="n">
+        <v>-240.2385419770698</v>
+      </c>
+      <c r="B116" t="n">
+        <v>-5.894052803576358</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="n">
+        <v>-237.2289830910518</v>
+      </c>
+      <c r="B117" t="n">
+        <v>-5.748975998851222</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="n">
+        <v>-234.2134252808547</v>
+      </c>
+      <c r="B118" t="n">
+        <v>-5.605582809578664</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="n">
+        <v>-231.1919514667755</v>
+      </c>
+      <c r="B119" t="n">
+        <v>-5.463882842653931</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="n">
+        <v>-228.1646109354797</v>
+      </c>
+      <c r="B120" t="n">
+        <v>-5.323884027284123</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="n">
+        <v>-225.1314981001225</v>
+      </c>
+      <c r="B121" t="n">
+        <v>-5.185596291592503</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="n">
+        <v>-222.0926847338356</v>
+      </c>
+      <c r="B122" t="n">
+        <v>-5.049028390473126</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="n">
+        <v>-219.0482488663033</v>
+      </c>
+      <c r="B123" t="n">
+        <v>-4.914189250210313</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="n">
+        <v>-215.998244955797</v>
+      </c>
+      <c r="B124" t="n">
+        <v>-4.781086655525399</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="n">
+        <v>-212.9427628486621</v>
+      </c>
+      <c r="B125" t="n">
+        <v>-4.649729842592109</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="n">
+        <v>-209.8818797768167</v>
+      </c>
+      <c r="B126" t="n">
+        <v>-4.520127366379711</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="n">
+        <v>-206.8156679257702</v>
+      </c>
+      <c r="B127" t="n">
+        <v>-4.39228745432888</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="n">
+        <v>-203.7441835023594</v>
+      </c>
+      <c r="B128" t="n">
+        <v>-4.266217577550918</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="n">
+        <v>-200.6675320115318</v>
+      </c>
+      <c r="B129" t="n">
+        <v>-4.141927119627837</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="n">
+        <v>-197.5857637168321</v>
+      </c>
+      <c r="B130" t="n">
+        <v>-4.01942309290925</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="n">
+        <v>-194.4989794359595</v>
+      </c>
+      <c r="B131" t="n">
+        <v>-3.898714422383932</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="n">
+        <v>-191.4072293199507</v>
+      </c>
+      <c r="B132" t="n">
+        <v>-3.779807919715751</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="n">
+        <v>-188.3106027927361</v>
+      </c>
+      <c r="B133" t="n">
+        <v>-3.662711820846994</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n">
+        <v>-185.2091784342015</v>
+      </c>
+      <c r="B134" t="n">
+        <v>-3.547433811334429</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="n">
+        <v>-182.1030297628303</v>
+      </c>
+      <c r="B135" t="n">
+        <v>-3.433981270654925</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="n">
+        <v>-178.9922288614686</v>
+      </c>
+      <c r="B136" t="n">
+        <v>-3.322361417540719</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n">
+        <v>-175.8768551927111</v>
+      </c>
+      <c r="B137" t="n">
+        <v>-3.212581622475057</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="n">
+        <v>-172.7569925262934</v>
+      </c>
+      <c r="B138" t="n">
+        <v>-3.104649278478405</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="n">
+        <v>-169.632709302172</v>
+      </c>
+      <c r="B139" t="n">
+        <v>-2.998571126336913</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="n">
+        <v>-166.5040897679807</v>
+      </c>
+      <c r="B140" t="n">
+        <v>-2.894354331815038</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="n">
+        <v>-163.3712128245132</v>
+      </c>
+      <c r="B141" t="n">
+        <v>-2.792005749817804</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="n">
+        <v>-160.2341520385412</v>
+      </c>
+      <c r="B142" t="n">
+        <v>-2.691531942010727</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="n">
+        <v>-157.0929756547999</v>
+      </c>
+      <c r="B143" t="n">
+        <v>-2.592939194360838</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="n">
+        <v>-153.94779111409</v>
+      </c>
+      <c r="B144" t="n">
+        <v>-2.496234889403752</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="n">
+        <v>-150.798649431139</v>
+      </c>
+      <c r="B145" t="n">
+        <v>-2.40142453042148</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="1" t="n">
+        <v>-147.6456362388753</v>
+      </c>
+      <c r="B146" t="n">
+        <v>-2.308514577709957</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="n">
+        <v>-144.4888418219402</v>
+      </c>
+      <c r="B147" t="n">
+        <v>-2.217511482693027</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="n">
+        <v>-141.3283348823309</v>
+      </c>
+      <c r="B148" t="n">
+        <v>-2.128420941446848</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="n">
+        <v>-138.1642007349489</v>
+      </c>
+      <c r="B149" t="n">
+        <v>-2.041249004448986</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="n">
+        <v>-134.9965025971995</v>
+      </c>
+      <c r="B150" t="n">
+        <v>-1.956000993304826</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="1" t="n">
+        <v>-131.8253535333198</v>
+      </c>
+      <c r="B151" t="n">
+        <v>-1.872683439914397</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="1" t="n">
+        <v>-128.6508061120787</v>
+      </c>
+      <c r="B152" t="n">
+        <v>-1.791301131674061</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="1" t="n">
+        <v>-125.4729511277737</v>
+      </c>
+      <c r="B153" t="n">
+        <v>-1.711859742828807</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="1" t="n">
+        <v>-122.2918634939859</v>
+      </c>
+      <c r="B154" t="n">
+        <v>-1.634364410411962</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="1" t="n">
+        <v>-119.1076177033884</v>
+      </c>
+      <c r="B155" t="n">
+        <v>-1.55882014723403</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="1" t="n">
+        <v>-115.9203109471446</v>
+      </c>
+      <c r="B156" t="n">
+        <v>-1.485232369817226</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="1" t="n">
+        <v>-112.7300235161008</v>
+      </c>
+      <c r="B157" t="n">
+        <v>-1.413605949061804</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="1" t="n">
+        <v>-109.5368245007582</v>
+      </c>
+      <c r="B158" t="n">
+        <v>-1.343945386499087</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="1" t="n">
+        <v>-106.3408005048322</v>
+      </c>
+      <c r="B159" t="n">
+        <v>-1.276255449512462</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="1" t="n">
+        <v>-103.142031577803</v>
+      </c>
+      <c r="B160" t="n">
+        <v>-1.210540628371746</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="1" t="n">
+        <v>-99.94060469410563</v>
+      </c>
+      <c r="B161" t="n">
+        <v>-1.14680542135099</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="1" t="n">
+        <v>-96.73660004929748</v>
+      </c>
+      <c r="B162" t="n">
+        <v>-1.085054052631961</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="1" t="n">
+        <v>-93.5300984016724</v>
+      </c>
+      <c r="B163" t="n">
+        <v>-1.025290628474238</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="1" t="n">
+        <v>-90.32116442197903</v>
+      </c>
+      <c r="B164" t="n">
+        <v>-0.9675188406175721</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="1" t="n">
+        <v>-87.10991203455781</v>
+      </c>
+      <c r="B165" t="n">
+        <v>-0.9117431327728696</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="1" t="n">
+        <v>-83.89640579919909</v>
+      </c>
+      <c r="B166" t="n">
+        <v>-0.8579669232404399</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="1" t="n">
+        <v>-80.6807321264113</v>
+      </c>
+      <c r="B167" t="n">
+        <v>-0.8061938870019674</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="1" t="n">
+        <v>-77.46296672332174</v>
+      </c>
+      <c r="B168" t="n">
+        <v>-0.7564273925291616</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="1" t="n">
+        <v>-74.24320218522362</v>
+      </c>
+      <c r="B169" t="n">
+        <v>-0.7086709367409867</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="1" t="n">
+        <v>-71.02151365403114</v>
+      </c>
+      <c r="B170" t="n">
+        <v>-0.6629276140602656</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="1" t="n">
+        <v>-67.79799382813553</v>
+      </c>
+      <c r="B171" t="n">
+        <v>-0.6192006362325628</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="1" t="n">
+        <v>-64.57271303910613</v>
+      </c>
+      <c r="B172" t="n">
+        <v>-0.5774927722343648</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="1" t="n">
+        <v>-61.34576923160873</v>
+      </c>
+      <c r="B173" t="n">
+        <v>-0.537807018976622</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="1" t="n">
+        <v>-58.11722702874166</v>
+      </c>
+      <c r="B174" t="n">
+        <v>-0.5001458210287524</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="1" t="n">
+        <v>-54.88717953152653</v>
+      </c>
+      <c r="B175" t="n">
+        <v>-0.4645118396646239</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="1" t="n">
+        <v>-51.65571340212911</v>
+      </c>
+      <c r="B176" t="n">
+        <v>-0.4309075098392441</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="1" t="n">
+        <v>-48.42291578159255</v>
+      </c>
+      <c r="B177" t="n">
+        <v>-0.3993351261464397</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="1" t="n">
+        <v>-45.18886288579929</v>
+      </c>
+      <c r="B178" t="n">
+        <v>-0.3697967404586393</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="1" t="n">
+        <v>-41.95363075890409</v>
+      </c>
+      <c r="B179" t="n">
+        <v>-0.3422942847170134</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="1" t="n">
+        <v>-38.71731782843555</v>
+      </c>
+      <c r="B180" t="n">
+        <v>-0.3168297422608077</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="1" t="n">
+        <v>-35.47999999152064</v>
+      </c>
+      <c r="B181" t="n">
+        <v>-0.293404765358332</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="1" t="n">
+        <v>-32.24176477528384</v>
+      </c>
+      <c r="B182" t="n">
+        <v>-0.2720209618460956</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="1" t="n">
+        <v>-29.00269951719753</v>
+      </c>
+      <c r="B183" t="n">
+        <v>-0.2526797913228904</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="1" t="n">
+        <v>-25.76288020559103</v>
+      </c>
+      <c r="B184" t="n">
+        <v>-0.2353825094181161</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="1" t="n">
+        <v>-22.52239464988883</v>
+      </c>
+      <c r="B185" t="n">
+        <v>-0.2201303059215149</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="1" t="n">
+        <v>-19.28132425438637</v>
+      </c>
+      <c r="B186" t="n">
+        <v>-0.2069241984826533</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="1" t="n">
+        <v>-16.03975665294326</v>
+      </c>
+      <c r="B187" t="n">
+        <v>-0.1957650926262033</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="1" t="n">
+        <v>-12.79777370422316</v>
+      </c>
+      <c r="B188" t="n">
+        <v>-0.1866537318783799</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="1" t="n">
+        <v>-9.555462648528653</v>
+      </c>
+      <c r="B189" t="n">
+        <v>-0.1795907370114662</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="1" t="n">
+        <v>-6.312900208843121</v>
+      </c>
+      <c r="B190" t="n">
+        <v>-0.1745765691465522</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="1" t="n">
+        <v>-3.070179010875414</v>
+      </c>
+      <c r="B191" t="n">
+        <v>-0.1716115793373945</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="1" t="n">
+        <v>0.1726244192368247</v>
+      </c>
+      <c r="B192" t="n">
+        <v>-0.1706959587311303</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="1" t="n">
+        <v>3.415411663158736</v>
+      </c>
+      <c r="B193" t="n">
+        <v>-0.1718297649463238</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="1" t="n">
+        <v>6.658117346879786</v>
+      </c>
+      <c r="B194" t="n">
+        <v>-0.175012923027424</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="1" t="n">
+        <v>9.90064284615241</v>
+      </c>
+      <c r="B195" t="n">
+        <v>-0.1802452033333566</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="1" t="n">
+        <v>13.14290648217114</v>
+      </c>
+      <c r="B196" t="n">
+        <v>-0.1875262440039194</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="1" t="n">
+        <v>16.38483174432102</v>
+      </c>
+      <c r="B197" t="n">
+        <v>-0.196855567121446</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="1" t="n">
+        <v>19.62632581795809</v>
+      </c>
+      <c r="B198" t="n">
+        <v>-0.2082325133874576</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="1" t="n">
+        <v>22.86731200655376</v>
+      </c>
+      <c r="B199" t="n">
+        <v>-0.2216563344108522</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="1" t="n">
+        <v>26.10769236313056</v>
+      </c>
+      <c r="B200" t="n">
+        <v>-0.2371260542738014</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="1" t="n">
+        <v>29.34740675661478</v>
+      </c>
+      <c r="B201" t="n">
+        <v>-0.254640739091144</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="1" t="n">
+        <v>32.58634053499418</v>
+      </c>
+      <c r="B202" t="n">
+        <v>-0.2741990317437057</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="1" t="n">
+        <v>35.82443382581928</v>
+      </c>
+      <c r="B203" t="n">
+        <v>-0.2957997409030781</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="1" t="n">
+        <v>39.06159371452812</v>
+      </c>
+      <c r="B204" t="n">
+        <v>-0.3194413469250321</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="1" t="n">
+        <v>42.29774406633911</v>
+      </c>
+      <c r="B205" t="n">
+        <v>-0.3451223074991105</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="1" t="n">
+        <v>45.53279223664642</v>
+      </c>
+      <c r="B206" t="n">
+        <v>-0.3728408155805596</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="1" t="n">
+        <v>48.7666507646181</v>
+      </c>
+      <c r="B207" t="n">
+        <v>-0.4025949532714321</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="1" t="n">
+        <v>51.99924383484117</v>
+      </c>
+      <c r="B208" t="n">
+        <v>-0.434382773652203</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="1" t="n">
+        <v>55.23048405955573</v>
+      </c>
+      <c r="B209" t="n">
+        <v>-0.4682020877254729</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="1" t="n">
+        <v>58.46029549295852</v>
+      </c>
+      <c r="B210" t="n">
+        <v>-0.5040506901052311</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="1" t="n">
+        <v>61.68858545058891</v>
+      </c>
+      <c r="B211" t="n">
+        <v>-0.5419260563030832</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="1" t="n">
+        <v>64.91526710129963</v>
+      </c>
+      <c r="B212" t="n">
+        <v>-0.5818255757442046</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="1" t="n">
+        <v>68.14028099928345</v>
+      </c>
+      <c r="B213" t="n">
+        <v>-0.6237468565809365</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="1" t="n">
+        <v>71.36351240950681</v>
+      </c>
+      <c r="B214" t="n">
+        <v>-0.6676866610234811</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="1" t="n">
+        <v>74.58489683528974</v>
+      </c>
+      <c r="B215" t="n">
+        <v>-0.7136422667572333</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="1" t="n">
+        <v>77.8043474289781</v>
+      </c>
+      <c r="B216" t="n">
+        <v>-0.7616105231926724</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="1" t="n">
+        <v>81.02178838722844</v>
+      </c>
+      <c r="B217" t="n">
+        <v>-0.8115883092410172</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="1" t="n">
+        <v>84.2371165914775</v>
+      </c>
+      <c r="B218" t="n">
+        <v>-0.8635719368423906</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="1" t="n">
+        <v>87.45027273423894</v>
+      </c>
+      <c r="B219" t="n">
+        <v>-0.9175582804590476</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="1" t="n">
+        <v>90.66115919152863</v>
+      </c>
+      <c r="B220" t="n">
+        <v>-0.9735434597093615</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="1" t="n">
+        <v>93.86970063842406</v>
+      </c>
+      <c r="B221" t="n">
+        <v>-1.031523831244868</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="1" t="n">
+        <v>97.07581620479144</v>
+      </c>
+      <c r="B222" t="n">
+        <v>-1.091495530343423</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="1" t="n">
+        <v>100.2794192210509</v>
+      </c>
+      <c r="B223" t="n">
+        <v>-1.153454448407075</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="1" t="n">
+        <v>103.4804291893521</v>
+      </c>
+      <c r="B224" t="n">
+        <v>-1.217396457262367</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="1" t="n">
+        <v>106.6787652061484</v>
+      </c>
+      <c r="B225" t="n">
+        <v>-1.283317291217855</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="1" t="n">
+        <v>109.8743520786866</v>
+      </c>
+      <c r="B226" t="n">
+        <v>-1.351212677634805</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="1" t="n">
+        <v>113.0670869690388</v>
+      </c>
+      <c r="B227" t="n">
+        <v>-1.421077615236612</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="1" t="n">
+        <v>116.2569063622722</v>
+      </c>
+      <c r="B228" t="n">
+        <v>-1.492907814199924</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="1" t="n">
+        <v>119.4437294049244</v>
+      </c>
+      <c r="B229" t="n">
+        <v>-1.566698492382102</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="1" t="n">
+        <v>122.627476075345</v>
+      </c>
+      <c r="B230" t="n">
+        <v>-1.642444758004302</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="1" t="n">
+        <v>125.8080602686188</v>
+      </c>
+      <c r="B231" t="n">
+        <v>-1.720141441239292</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="1" t="n">
+        <v>128.9853961997616</v>
+      </c>
+      <c r="B232" t="n">
+        <v>-1.799783237309811</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" s="1" t="n">
+        <v>132.1594149016205</v>
+      </c>
+      <c r="B233" t="n">
+        <v>-1.881365136523243</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" s="1" t="n">
+        <v>135.330025351238</v>
+      </c>
+      <c r="B234" t="n">
+        <v>-1.964881442380403</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" s="1" t="n">
+        <v>138.4971530917165</v>
+      </c>
+      <c r="B235" t="n">
+        <v>-2.050326754735806</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" s="1" t="n">
+        <v>141.6607123961695</v>
+      </c>
+      <c r="B236" t="n">
+        <v>-2.137695245648672</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" s="1" t="n">
+        <v>144.820640354314</v>
+      </c>
+      <c r="B237" t="n">
+        <v>-2.226981596742377</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" s="1" t="n">
+        <v>147.9768462771784</v>
+      </c>
+      <c r="B238" t="n">
+        <v>-2.318179595213422</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" s="1" t="n">
+        <v>151.1292444045843</v>
+      </c>
+      <c r="B239" t="n">
+        <v>-2.411283020672641</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" s="1" t="n">
+        <v>154.2777669804787</v>
+      </c>
+      <c r="B240" t="n">
+        <v>-2.506286059535967</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" s="1" t="n">
+        <v>157.4223284166665</v>
+      </c>
+      <c r="B241" t="n">
+        <v>-2.603182247663483</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" s="1" t="n">
+        <v>160.5628497490364</v>
+      </c>
+      <c r="B242" t="n">
+        <v>-2.701965189895162</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" s="1" t="n">
+        <v>163.6992515400972</v>
+      </c>
+      <c r="B243" t="n">
+        <v>-2.802628351394532</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" s="1" t="n">
+        <v>166.8314655917337</v>
+      </c>
+      <c r="B244" t="n">
+        <v>-2.905165443081074</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" s="1" t="n">
+        <v>169.9593960560591</v>
+      </c>
+      <c r="B245" t="n">
+        <v>-3.00956914821171</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" s="1" t="n">
+        <v>173.0829918163692</v>
+      </c>
+      <c r="B246" t="n">
+        <v>-3.115833517686212</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" s="1" t="n">
+        <v>176.202157502594</v>
+      </c>
+      <c r="B247" t="n">
+        <v>-3.223951002559204</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" s="1" t="n">
+        <v>179.3168080734908</v>
+      </c>
+      <c r="B248" t="n">
+        <v>-3.333914255539781</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" s="1" t="n">
+        <v>182.4268818502251</v>
+      </c>
+      <c r="B249" t="n">
+        <v>-3.445716636594938</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" s="1" t="n">
+        <v>185.5322891330504</v>
+      </c>
+      <c r="B250" t="n">
+        <v>-3.559350392536373</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" s="1" t="n">
+        <v>188.6329678489116</v>
+      </c>
+      <c r="B251" t="n">
+        <v>-3.674808655689333</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" s="1" t="n">
+        <v>191.7288284647445</v>
+      </c>
+      <c r="B252" t="n">
+        <v>-3.792083429760481</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" s="1" t="n">
+        <v>194.8198033312801</v>
+      </c>
+      <c r="B253" t="n">
+        <v>-3.911167417141229</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" s="1" t="n">
+        <v>197.9058030605296</v>
+      </c>
+      <c r="B254" t="n">
+        <v>-4.032052367804994</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" s="1" t="n">
+        <v>200.986766607871</v>
+      </c>
+      <c r="B255" t="n">
+        <v>-4.154731018465782</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" s="1" t="n">
+        <v>204.0626150384</v>
+      </c>
+      <c r="B256" t="n">
+        <v>-4.279195299259641</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" s="1" t="n">
+        <v>207.1332711236202</v>
+      </c>
+      <c r="B257" t="n">
+        <v>-4.40543708791364</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" s="1" t="n">
+        <v>210.1986560728325</v>
+      </c>
+      <c r="B258" t="n">
+        <v>-4.533448077626247</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" s="1" t="n">
+        <v>213.2586979680641</v>
+      </c>
+      <c r="B259" t="n">
+        <v>-4.66322013242484</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" s="1" t="n">
+        <v>216.3133297967842</v>
+      </c>
+      <c r="B260" t="n">
+        <v>-4.79474522433074</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" s="1" t="n">
+        <v>219.362451745146</v>
+      </c>
+      <c r="B261" t="n">
+        <v>-4.928013789802264</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" s="1" t="n">
+        <v>222.4060195661466</v>
+      </c>
+      <c r="B262" t="n">
+        <v>-5.063018569883582</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" s="1" t="n">
+        <v>225.4439500566386</v>
+      </c>
+      <c r="B263" t="n">
+        <v>-5.199750508071787</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" s="1" t="n">
+        <v>228.4761600614436</v>
+      </c>
+      <c r="B264" t="n">
+        <v>-5.338200416463366</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" s="1" t="n">
+        <v>231.5025771072486</v>
+      </c>
+      <c r="B265" t="n">
+        <v>-5.478359471532656</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" s="1" t="n">
+        <v>234.5231415798937</v>
+      </c>
+      <c r="B266" t="n">
+        <v>-5.620219352209944</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" s="1" t="n">
+        <v>237.5377643147674</v>
+      </c>
+      <c r="B267" t="n">
+        <v>-5.763770249532115</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" s="1" t="n">
+        <v>240.5463792746585</v>
+      </c>
+      <c r="B268" t="n">
+        <v>-5.90900332918838</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" s="1" t="n">
+        <v>243.5489150021525</v>
+      </c>
+      <c r="B269" t="n">
+        <v>-6.055909401842058</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" s="1" t="n">
+        <v>246.5452942253401</v>
+      </c>
+      <c r="B270" t="n">
+        <v>-6.2044788858706</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" s="1" t="n">
+        <v>249.5354511303664</v>
+      </c>
+      <c r="B271" t="n">
+        <v>-6.35470266146973</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" s="1" t="n">
+        <v>252.5193085606271</v>
+      </c>
+      <c r="B272" t="n">
+        <v>-6.506570941111676</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" s="1" t="n">
+        <v>255.4967949236708</v>
+      </c>
+      <c r="B273" t="n">
+        <v>-6.660074108956252</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" s="1" t="n">
+        <v>258.4678449780558</v>
+      </c>
+      <c r="B274" t="n">
+        <v>-6.815202781045201</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" s="1" t="n">
+        <v>261.432369871483</v>
+      </c>
+      <c r="B275" t="n">
+        <v>-6.971946232787076</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" s="1" t="n">
+        <v>264.3903159177707</v>
+      </c>
+      <c r="B276" t="n">
+        <v>-7.130295485834978</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" s="1" t="n">
+        <v>267.3416002550832</v>
+      </c>
+      <c r="B277" t="n">
+        <v>-7.29023991780582</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" s="1" t="n">
+        <v>270.2861689477417</v>
+      </c>
+      <c r="B278" t="n">
+        <v>-7.451770371089481</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" s="1" t="n">
+        <v>273.2239332434033</v>
+      </c>
+      <c r="B279" t="n">
+        <v>-7.614875690311578</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" s="1" t="n">
+        <v>276.154828587243</v>
+      </c>
+      <c r="B280" t="n">
+        <v>-7.779545940809072</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" s="1" t="n">
+        <v>279.0787829072635</v>
+      </c>
+      <c r="B281" t="n">
+        <v>-7.945770676642752</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" s="1" t="n">
+        <v>281.9957317365922</v>
+      </c>
+      <c r="B282" t="n">
+        <v>-8.113539790110792</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" s="1" t="n">
+        <v>284.9055918987527</v>
+      </c>
+      <c r="B283" t="n">
+        <v>-8.282841998269703</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" s="1" t="n">
+        <v>287.8083161147878</v>
+      </c>
+      <c r="B284" t="n">
+        <v>-8.453668011380017</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" s="1" t="n">
+        <v>290.7038092352855</v>
+      </c>
+      <c r="B285" t="n">
+        <v>-8.626005641038006</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" s="1" t="n">
+        <v>293.5920120286447</v>
+      </c>
+      <c r="B286" t="n">
+        <v>-8.799844709932756</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" s="1" t="n">
+        <v>296.4728713317533</v>
+      </c>
+      <c r="B287" t="n">
+        <v>-8.975175346152952</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" s="1" t="n">
+        <v>299.3462979262456</v>
+      </c>
+      <c r="B288" t="n">
+        <v>-9.151985399068508</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" s="1" t="n">
+        <v>302.2122214277216</v>
+      </c>
+      <c r="B289" t="n">
+        <v>-9.330263749853259</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" s="1" t="n">
+        <v>305.0705822341291</v>
+      </c>
+      <c r="B290" t="n">
+        <v>-9.509999866427421</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" s="1" t="n">
+        <v>307.9213030597575</v>
+      </c>
+      <c r="B291" t="n">
+        <v>-9.69118202217993</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" s="1" t="n">
+        <v>310.7643242774222</v>
+      </c>
+      <c r="B292" t="n">
+        <v>-9.87379951768483</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" s="1" t="n">
+        <v>313.5995810821393</v>
+      </c>
+      <c r="B293" t="n">
+        <v>-10.05784125139124</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" s="1" t="n">
+        <v>316.4269956439912</v>
+      </c>
+      <c r="B294" t="n">
+        <v>-10.24329518542547</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" s="1" t="n">
+        <v>319.2464969959914</v>
+      </c>
+      <c r="B295" t="n">
+        <v>-10.43014962587876</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" s="1" t="n">
+        <v>322.0580314854702</v>
+      </c>
+      <c r="B296" t="n">
+        <v>-10.61839394971142</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" s="1" t="n">
+        <v>324.8615037164732</v>
+      </c>
+      <c r="B297" t="n">
+        <v>-10.80801465095831</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" s="1" t="n">
+        <v>327.6568721100469</v>
+      </c>
+      <c r="B298" t="n">
+        <v>-10.99900175805945</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" s="1" t="n">
+        <v>330.4440678885829</v>
+      </c>
+      <c r="B299" t="n">
+        <v>-11.1913434015766</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" s="1" t="n">
+        <v>333.2229953460098</v>
+      </c>
+      <c r="B300" t="n">
+        <v>-11.38502574095793</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" s="1" t="n">
+        <v>335.9936127723325</v>
+      </c>
+      <c r="B301" t="n">
+        <v>-11.58003859356722</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" s="1" t="n">
+        <v>338.7558686225206</v>
+      </c>
+      <c r="B302" t="n">
+        <v>-11.77637106438422</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" s="1" t="n">
+        <v>341.5096436761913</v>
+      </c>
+      <c r="B303" t="n">
+        <v>-11.97400734325214</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" s="1" t="n">
+        <v>344.2549073865875</v>
+      </c>
+      <c r="B304" t="n">
+        <v>-12.17293785009576</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" s="1" t="n">
+        <v>346.991587101889</v>
+      </c>
+      <c r="B305" t="n">
+        <v>-12.3731499343736</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" s="1" t="n">
+        <v>349.7196142534867</v>
+      </c>
+      <c r="B306" t="n">
+        <v>-12.57463115479791</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" s="1" t="n">
+        <v>352.4389121337685</v>
+      </c>
+      <c r="B307" t="n">
+        <v>-12.77736837969096</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" s="1" t="n">
+        <v>355.1494270926013</v>
+      </c>
+      <c r="B308" t="n">
+        <v>-12.98135011660534</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" s="1" t="n">
+        <v>357.8510801970496</v>
+      </c>
+      <c r="B309" t="n">
+        <v>-13.18656290666621</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" s="1" t="n">
+        <v>360.5438066382729</v>
+      </c>
+      <c r="B310" t="n">
+        <v>-13.39299427026265</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" s="1" t="n">
+        <v>363.2275428496633</v>
+      </c>
+      <c r="B311" t="n">
+        <v>-13.60063175638052</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" s="1" t="n">
+        <v>365.9022246532524</v>
+      </c>
+      <c r="B312" t="n">
+        <v>-13.80946280333541</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" s="1" t="n">
+        <v>368.567762831468</v>
+      </c>
+      <c r="B313" t="n">
+        <v>-14.01947280419165</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" s="1" t="n">
+        <v>371.2241263379426</v>
+      </c>
+      <c r="B314" t="n">
+        <v>-14.2306516613732</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" s="1" t="n">
+        <v>373.8712169187363</v>
+      </c>
+      <c r="B315" t="n">
+        <v>-14.4429838968008</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" s="1" t="n">
+        <v>376.5089724900613</v>
+      </c>
+      <c r="B316" t="n">
+        <v>-14.65645681327868</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" s="1" t="n">
+        <v>379.137336572072</v>
+      </c>
+      <c r="B317" t="n">
+        <v>-14.87105811881321</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" s="1" t="n">
+        <v>381.7562409308688</v>
+      </c>
+      <c r="B318" t="n">
+        <v>-15.08677451298539</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" s="1" t="n">
+        <v>384.3656011949115</v>
+      </c>
+      <c r="B319" t="n">
+        <v>-15.30359127979182</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" s="1" t="n">
+        <v>386.9653606749796</v>
+      </c>
+      <c r="B320" t="n">
+        <v>-15.521495918124</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" s="1" t="n">
+        <v>389.5554528331833</v>
+      </c>
+      <c r="B321" t="n">
+        <v>-15.74047505754706</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" s="1" t="n">
+        <v>392.1358021354193</v>
+      </c>
+      <c r="B322" t="n">
+        <v>-15.96051449702213</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" s="1" t="n">
+        <v>394.7063540947545</v>
+      </c>
+      <c r="B323" t="n">
+        <v>-16.18160176750058</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" s="1" t="n">
+        <v>397.2670258638165</v>
+      </c>
+      <c r="B324" t="n">
+        <v>-16.40372190827605</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" s="1" t="n">
+        <v>399.8177536362505</v>
+      </c>
+      <c r="B325" t="n">
+        <v>-16.62686152667536</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" s="1" t="n">
+        <v>402.3584685722021</v>
+      </c>
+      <c r="B326" t="n">
+        <v>-16.85100673823592</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" s="1" t="n">
+        <v>404.8890949892802</v>
+      </c>
+      <c r="B327" t="n">
+        <v>-17.07614298765287</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" s="1" t="n">
+        <v>407.4095785715107</v>
+      </c>
+      <c r="B328" t="n">
+        <v>-17.30225756619771</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" s="1" t="n">
+        <v>409.919845040956</v>
+      </c>
+      <c r="B329" t="n">
+        <v>-17.52933593975706</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" s="1" t="n">
+        <v>412.419822252892</v>
+      </c>
+      <c r="B330" t="n">
+        <v>-17.75736369988815</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" s="1" t="n">
+        <v>414.9094283812789</v>
+      </c>
+      <c r="B331" t="n">
+        <v>-17.98632548271763</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" s="1" t="n">
+        <v>417.3886151257879</v>
+      </c>
+      <c r="B332" t="n">
+        <v>-18.21620895585957</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" s="1" t="n">
+        <v>419.8573004022459</v>
+      </c>
+      <c r="B333" t="n">
+        <v>-18.4469986322209</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" s="1" t="n">
+        <v>422.3154161322108</v>
+      </c>
+      <c r="B334" t="n">
+        <v>-18.67868026445052</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" s="1" t="n">
+        <v>424.7628986063081</v>
+      </c>
+      <c r="B335" t="n">
+        <v>-18.91123998237774</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" s="1" t="n">
+        <v>427.1996572789531</v>
+      </c>
+      <c r="B336" t="n">
+        <v>-19.14466131186043</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" s="1" t="n">
+        <v>429.6256391806845</v>
+      </c>
+      <c r="B337" t="n">
+        <v>-19.37893131719929</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" s="1" t="n">
+        <v>432.0407666402733</v>
+      </c>
+      <c r="B338" t="n">
+        <v>-19.6140346648705</v>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" s="1" t="n">
+        <v>434.4449663148073</v>
+      </c>
+      <c r="B339" t="n">
+        <v>-19.84995639005726</v>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" s="1" t="n">
+        <v>436.8381691514398</v>
+      </c>
+      <c r="B340" t="n">
+        <v>-20.08668191261995</v>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" s="1" t="n">
+        <v>439.2203018709669</v>
+      </c>
+      <c r="B341" t="n">
+        <v>-20.32419620551451</v>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" s="1" t="n">
+        <v>441.5913002893877</v>
+      </c>
+      <c r="B342" t="n">
+        <v>-20.56248512571966</v>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" s="1" t="n">
+        <v>443.9510809016919</v>
+      </c>
+      <c r="B343" t="n">
+        <v>-20.8015325650257</v>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" s="1" t="n">
+        <v>446.2995692755619</v>
+      </c>
+      <c r="B344" t="n">
+        <v>-21.0413232871046</v>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" s="1" t="n">
+        <v>448.6367001382736</v>
+      </c>
+      <c r="B345" t="n">
+        <v>-21.28184297672107</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" s="1" t="n">
+        <v>450.9624048621395</v>
+      </c>
+      <c r="B346" t="n">
+        <v>-21.52307697903214</v>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" s="1" t="n">
+        <v>453.2765919478367</v>
+      </c>
+      <c r="B347" t="n">
+        <v>-21.76500824360932</v>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" s="1" t="n">
+        <v>455.5791954891408</v>
+      </c>
+      <c r="B348" t="n">
+        <v>-22.00762236082335</v>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" s="1" t="n">
+        <v>457.8701455325519</v>
+      </c>
+      <c r="B349" t="n">
+        <v>-22.2509045134876</v>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" s="1" t="n">
+        <v>460.1493750065135</v>
+      </c>
+      <c r="B350" t="n">
+        <v>-22.4948402111157</v>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" s="1" t="n">
+        <v>462.4167922057921</v>
+      </c>
+      <c r="B351" t="n">
+        <v>-22.73941232961241</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" s="1" t="n">
+        <v>464.6723354806541</v>
+      </c>
+      <c r="B352" t="n">
+        <v>-22.98460698155566</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" s="1" t="n">
+        <v>466.9159344974843</v>
+      </c>
+      <c r="B353" t="n">
+        <v>-23.23040939034865</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" s="1" t="n">
+        <v>469.1474963314266</v>
+      </c>
+      <c r="B354" t="n">
+        <v>-23.47680232132336</v>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" s="1" t="n">
+        <v>471.366963288048</v>
+      </c>
+      <c r="B355" t="n">
+        <v>-23.72377244926514</v>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" s="1" t="n">
+        <v>473.5742486517984</v>
+      </c>
+      <c r="B356" t="n">
+        <v>-23.97130328919479</v>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" s="1" t="n">
+        <v>475.7692884234614</v>
+      </c>
+      <c r="B357" t="n">
+        <v>-24.21938094740122</v>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" s="1" t="n">
+        <v>477.9519993870979</v>
+      </c>
+      <c r="B358" t="n">
+        <v>-24.46798943879043</v>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" s="1" t="n">
+        <v>480.1223246090354</v>
+      </c>
+      <c r="B359" t="n">
+        <v>-24.71711585415602</v>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" s="1" t="n">
+        <v>482.2801950662918</v>
+      </c>
+      <c r="B360" t="n">
+        <v>-24.96674603524787</v>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" s="1" t="n">
+        <v>484.4255098496301</v>
+      </c>
+      <c r="B361" t="n">
+        <v>-25.21686221767368</v>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" s="1" t="n">
+        <v>486.5582237704055</v>
+      </c>
+      <c r="B362" t="n">
+        <v>-25.46745323010077</v>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" s="1" t="n">
+        <v>488.6782505794302</v>
+      </c>
+      <c r="B363" t="n">
+        <v>-25.71850326295043</v>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" s="1" t="n">
+        <v>490.7855347812896</v>
+      </c>
+      <c r="B364" t="n">
+        <v>-25.97000029715102</v>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" s="1" t="n">
+        <v>492.8800095788409</v>
+      </c>
+      <c r="B365" t="n">
+        <v>-26.22193118886997</v>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" s="1" t="n">
+        <v>494.961606367523</v>
+      </c>
+      <c r="B366" t="n">
+        <v>-26.47428279183995</v>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" s="1" t="n">
+        <v>497.0302626045175</v>
+      </c>
+      <c r="B367" t="n">
+        <v>-26.72704293500914</v>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" s="1" t="n">
+        <v>499.0859352644209</v>
+      </c>
+      <c r="B368" t="n">
+        <v>-26.98020213862799</v>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" s="1" t="n">
+        <v>501.128550796317</v>
+      </c>
+      <c r="B369" t="n">
+        <v>-27.23374750091972</v>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" s="1" t="n">
+        <v>503.1580634223577</v>
+      </c>
+      <c r="B370" t="n">
+        <v>-27.48766989809937</v>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" s="1" t="n">
+        <v>505.1744147975543</v>
+      </c>
+      <c r="B371" t="n">
+        <v>-27.7419590465278</v>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" s="1" t="n">
+        <v>507.1775826033028</v>
+      </c>
+      <c r="B372" t="n">
+        <v>-27.996609674826</v>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" s="1" t="n">
+        <v>509.1675273085694</v>
+      </c>
+      <c r="B373" t="n">
+        <v>-28.25161489819328</v>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" s="1" t="n">
+        <v>511.1442133936517</v>
+      </c>
+      <c r="B374" t="n">
+        <v>-28.50696892591463</v>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" s="1" t="n">
+        <v>513.1076383016425</v>
+      </c>
+      <c r="B375" t="n">
+        <v>-28.76267091426166</v>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" s="1" t="n">
+        <v>515.0577754858793</v>
+      </c>
+      <c r="B376" t="n">
+        <v>-29.01871768894986</v>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" s="1" t="n">
+        <v>516.9946418144401</v>
+      </c>
+      <c r="B377" t="n">
+        <v>-29.2751126340552</v>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" s="1" t="n">
+        <v>518.9182618923427</v>
+      </c>
+      <c r="B378" t="n">
+        <v>-29.53186121543803</v>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" s="1" t="n">
+        <v>520.8286672211713</v>
+      </c>
+      <c r="B379" t="n">
+        <v>-29.78897098893998</v>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" s="1" t="n">
+        <v>522.7259058166068</v>
+      </c>
+      <c r="B380" t="n">
+        <v>-30.04645303784031</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" s="1" t="n">
+        <v>524.6100786912355</v>
+      </c>
+      <c r="B381" t="n">
+        <v>-30.30432717970746</v>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" s="1" t="n">
+        <v>526.4812762673264</v>
+      </c>
+      <c r="B382" t="n">
+        <v>-30.56261357842527</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding the reflections, vectors
</commit_message>
<xml_diff>
--- a/Phase_distribution_0.xlsx
+++ b/Phase_distribution_0.xlsx
@@ -440,3050 +440,3050 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>-526.3472030509745</v>
+        <v>-526.3209500055157</v>
       </c>
       <c r="B2" t="n">
-        <v>-30.54403340524266</v>
+        <v>-30.540395117831</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>-524.4736779913088</v>
+        <v>-524.4479470372619</v>
       </c>
       <c r="B3" t="n">
-        <v>-30.28558534772463</v>
+        <v>-30.28204973086</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>-522.5872033986449</v>
+        <v>-522.5619826905364</v>
       </c>
       <c r="B4" t="n">
-        <v>-30.02755566708299</v>
+        <v>-30.02411935436305</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>-520.6876946775437</v>
+        <v>-520.662931608397</v>
       </c>
       <c r="B5" t="n">
-        <v>-29.76992492741658</v>
+        <v>-29.76657914946242</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>-518.7750457116435</v>
+        <v>-518.7507575836784</v>
       </c>
       <c r="B6" t="n">
-        <v>-29.51267254726389</v>
+        <v>-29.50941813239587</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>-516.8492212102877</v>
+        <v>-516.8253772395135</v>
       </c>
       <c r="B7" t="n">
-        <v>-29.25578906989051</v>
+        <v>-29.25262045067518</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>-514.9101674327534</v>
+        <v>-514.8867386148538</v>
       </c>
       <c r="B8" t="n">
-        <v>-28.99926390209771</v>
+        <v>-28.99617589323498</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>-512.9578688082988</v>
+        <v>-512.9348661186879</v>
       </c>
       <c r="B9" t="n">
-        <v>-28.74309272472178</v>
+        <v>-28.74008549947851</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>-510.9923110681352</v>
+        <v>-510.96971159504</v>
       </c>
       <c r="B10" t="n">
-        <v>-28.48727242656781</v>
+        <v>-28.48434176895807</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>-509.0135058453289</v>
+        <v>-508.9913052284678</v>
       </c>
       <c r="B11" t="n">
-        <v>-28.23180419089238</v>
+        <v>-28.22894837662182</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>-507.021482121423</v>
+        <v>-506.9996563762015</v>
       </c>
       <c r="B12" t="n">
-        <v>-27.97669220664864</v>
+        <v>-27.97390705304349</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>-505.0162505185625</v>
+        <v>-504.9947869090348</v>
       </c>
       <c r="B13" t="n">
-        <v>-27.72193900510649</v>
+        <v>-27.71922185605064</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>-502.9978363153704</v>
+        <v>-502.9767566420569</v>
       </c>
       <c r="B14" t="n">
-        <v>-27.46754964961067</v>
+        <v>-27.46490224945555</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>-500.9663083704347</v>
+        <v>-500.9455843324719</v>
       </c>
       <c r="B15" t="n">
-        <v>-27.21353521949166</v>
+        <v>-27.21095303177219</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>-498.9216803158042</v>
+        <v>-498.9013113393704</v>
       </c>
       <c r="B16" t="n">
-        <v>-26.95990034360466</v>
+        <v>-26.95738236595901</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>-496.8640342401368</v>
+        <v>-496.8440001712912</v>
       </c>
       <c r="B17" t="n">
-        <v>-26.70665860204483</v>
+        <v>-26.70420145360481</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>-494.7934062370233</v>
+        <v>-494.7737074712043</v>
       </c>
       <c r="B18" t="n">
-        <v>-26.45381823716292</v>
+        <v>-26.45142111514548</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>-492.7098485792596</v>
+        <v>-492.6904892925363</v>
       </c>
       <c r="B19" t="n">
-        <v>-26.20138985102597</v>
+        <v>-26.1990524264196</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>-490.6134470420977</v>
+        <v>-490.5944085875326</v>
       </c>
       <c r="B20" t="n">
-        <v>-25.94938837611346</v>
+        <v>-25.94710759172716</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>-488.5042357404968</v>
+        <v>-488.485523249671</v>
       </c>
       <c r="B21" t="n">
-        <v>-25.69782277363902</v>
+        <v>-25.69559846689049</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>-486.3822983315987</v>
+        <v>-486.3639000992166</v>
       </c>
       <c r="B22" t="n">
-        <v>-25.44670818551924</v>
+        <v>-25.44453820935183</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>-484.2477089985559</v>
+        <v>-484.2296142165903</v>
       </c>
       <c r="B23" t="n">
-        <v>-25.19605878016785</v>
+        <v>-25.19394113883445</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>-482.1005046069063</v>
+        <v>-482.0827291540471</v>
       </c>
       <c r="B24" t="n">
-        <v>-24.94588454647533</v>
+        <v>-24.94382038515704</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>-479.940791521815</v>
+        <v>-479.923318309864</v>
       </c>
       <c r="B25" t="n">
-        <v>-24.69620374919211</v>
+        <v>-24.6941903850992</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>-477.7686217431812</v>
+        <v>-477.7514408685112</v>
       </c>
       <c r="B26" t="n">
-        <v>-24.44702844352523</v>
+        <v>-24.44506407349536</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>-475.5840738250679</v>
+        <v>-475.5671951964998</v>
       </c>
       <c r="B27" t="n">
-        <v>-24.19837388157708</v>
+        <v>-24.19645898586833</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>-473.3872141442815</v>
+        <v>-473.3706274944925</v>
       </c>
       <c r="B28" t="n">
-        <v>-23.95025402236999</v>
+        <v>-23.94838679597777</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>-471.1781124276358</v>
+        <v>-471.1618247999816</v>
       </c>
       <c r="B29" t="n">
-        <v>-23.70268330666292</v>
+        <v>-23.70086391424678</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>-468.9568674908161</v>
+        <v>-468.940872925242</v>
       </c>
       <c r="B30" t="n">
-        <v>-23.45567948327266</v>
+        <v>-23.45390663929405</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>-466.7235242997001</v>
+        <v>-466.7078104848711</v>
       </c>
       <c r="B31" t="n">
-        <v>-23.20925435443723</v>
+        <v>-23.20752610101636</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>-464.4781562687113</v>
+        <v>-464.462736640075</v>
       </c>
       <c r="B32" t="n">
-        <v>-22.96342297528892</v>
+        <v>-22.96174020249464</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>-462.2208691430645</v>
+        <v>-462.2057154767515</v>
       </c>
       <c r="B33" t="n">
-        <v>-22.71820394289267</v>
+        <v>-22.71656300574676</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>-459.9517071643301</v>
+        <v>-459.9368368608303</v>
       </c>
       <c r="B34" t="n">
-        <v>-22.47360917376716</v>
+        <v>-22.4720114059611</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>-457.6707503370602</v>
+        <v>-457.6561677880746</v>
       </c>
       <c r="B35" t="n">
-        <v>-22.22965451983504</v>
+        <v>-22.22809983268306</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>-455.3780719573454</v>
+        <v>-455.3637651849463</v>
       </c>
       <c r="B36" t="n">
-        <v>-21.98635512064564</v>
+        <v>-21.98484169125899</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>-453.0737604705545</v>
+        <v>-453.0597152692862</v>
       </c>
       <c r="B37" t="n">
-        <v>-21.74372771718336</v>
+        <v>-21.7422535250895</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>-450.7578668088418</v>
+        <v>-450.7441062658509</v>
       </c>
       <c r="B38" t="n">
-        <v>-21.50178510173038</v>
+        <v>-21.50035204915952</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>-448.4304887754113</v>
+        <v>-448.4169828563089</v>
       </c>
       <c r="B39" t="n">
-        <v>-21.26054498021159</v>
+        <v>-21.25914943378112</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>-446.0916757036269</v>
+        <v>-446.0784483024984</v>
       </c>
       <c r="B40" t="n">
-        <v>-21.02002000651123</v>
+        <v>-21.01866393663133</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>-443.7415254156298</v>
+        <v>-443.7285680464067</v>
       </c>
       <c r="B41" t="n">
-        <v>-20.78022783018451</v>
+        <v>-20.77890986339332</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>-441.3800931065904</v>
+        <v>-441.3673951192543</v>
       </c>
       <c r="B42" t="n">
-        <v>-20.54118170617224</v>
+        <v>-20.53990027745272</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>-439.0074496330629</v>
+        <v>-438.995019040299</v>
       </c>
       <c r="B43" t="n">
-        <v>-20.30289649384298</v>
+        <v>-20.30165193554342</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>-436.6236817881099</v>
+        <v>-436.6115107136291</v>
       </c>
       <c r="B44" t="n">
-        <v>-20.06538861661326</v>
+        <v>-20.06417966966356</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>-434.2288536155687</v>
+        <v>-434.216934671644</v>
       </c>
       <c r="B45" t="n">
-        <v>-19.82867218512735</v>
+        <v>-19.82749766232021</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>-431.8230288394137</v>
+        <v>-431.8113915930381</v>
       </c>
       <c r="B46" t="n">
-        <v>-19.59276127469559</v>
+        <v>-19.59162361993367</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>-429.4063016769393</v>
+        <v>-429.3949105346652</v>
       </c>
       <c r="B47" t="n">
-        <v>-19.35767290822088</v>
+        <v>-19.3565681869205</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>-426.9787196594624</v>
+        <v>-426.9675926260201</v>
       </c>
       <c r="B48" t="n">
-        <v>-19.12341951450946</v>
+        <v>-19.12234903125713</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>-424.5403765964429</v>
+        <v>-424.5295056155436</v>
       </c>
       <c r="B49" t="n">
-        <v>-18.89001797146497</v>
+        <v>-18.88898050781248</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>-422.0913193645184</v>
+        <v>-422.0806972971806</v>
       </c>
       <c r="B50" t="n">
-        <v>-18.65748060691388</v>
+        <v>-18.65647505438659</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>-419.6316430757205</v>
+        <v>-419.6212692187369</v>
       </c>
       <c r="B51" t="n">
-        <v>-18.42582430538087</v>
+        <v>-18.42485017858561</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>-417.161401175011</v>
+        <v>-417.151273553826</v>
       </c>
       <c r="B52" t="n">
-        <v>-18.19506195396451</v>
+        <v>-18.19411865486089</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>-414.6806595029104</v>
+        <v>-414.6708024864402</v>
       </c>
       <c r="B53" t="n">
-        <v>-17.96520758881886</v>
+        <v>-17.9642969581879</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>-412.1895111671856</v>
+        <v>-412.1798986416407</v>
       </c>
       <c r="B54" t="n">
-        <v>-17.73627770674813</v>
+        <v>-17.73539691250798</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>-409.6880034927844</v>
+        <v>-409.6786432714717</v>
       </c>
       <c r="B55" t="n">
-        <v>-17.50828452723346</v>
+        <v>-17.50743387972435</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>-407.1762211723109</v>
+        <v>-407.1671067576169</v>
       </c>
       <c r="B56" t="n">
-        <v>-17.28124364980434</v>
+        <v>-17.2804221562468</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>-404.6542299230811</v>
+        <v>-404.6453569094813</v>
       </c>
       <c r="B57" t="n">
-        <v>-17.05516888057554</v>
+        <v>-17.05437575251338</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>-402.1220960579145</v>
+        <v>-402.1134697778352</v>
       </c>
       <c r="B58" t="n">
-        <v>-16.83007403396198</v>
+        <v>-16.82930935775039</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>-399.5798876257906</v>
+        <v>-399.5715032431371</v>
       </c>
       <c r="B59" t="n">
-        <v>-16.60597302877568</v>
+        <v>-16.60523598899528</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>-397.0276689807418</v>
+        <v>-397.0195356616037</v>
       </c>
       <c r="B60" t="n">
-        <v>-16.38287940674704</v>
+        <v>-16.38217042031008</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>-394.4655298508153</v>
+        <v>-394.4576340006365</v>
       </c>
       <c r="B61" t="n">
-        <v>-16.16080885423938</v>
+        <v>-16.16012635527284</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>-391.8935101358704</v>
+        <v>-391.8858629321753</v>
       </c>
       <c r="B62" t="n">
-        <v>-15.93977266969756</v>
+        <v>-15.93911724542869</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>-389.3117038791105</v>
+        <v>-389.3042893209173</v>
       </c>
       <c r="B63" t="n">
-        <v>-15.71978676889586</v>
+        <v>-15.71915667779089</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>-386.7201601537267</v>
+        <v>-386.7129923121398</v>
       </c>
       <c r="B64" t="n">
-        <v>-15.50086314596476</v>
+        <v>-15.50025921369678</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>-384.1189631884458</v>
+        <v>-384.1120294816633</v>
       </c>
       <c r="B65" t="n">
-        <v>-15.28301671919758</v>
+        <v>-15.2824375201545</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>-381.5081678648841</v>
+        <v>-381.5014635421405</v>
       </c>
       <c r="B66" t="n">
-        <v>-15.06625986872137</v>
+        <v>-15.06570465431207</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>-378.8878458070191</v>
+        <v>-378.8813853470432</v>
       </c>
       <c r="B67" t="n">
-        <v>-14.85060631863783</v>
+        <v>-14.8500759282372</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>-376.2580717304365</v>
+        <v>-376.2518483921783</v>
       </c>
       <c r="B68" t="n">
-        <v>-14.63606996653718</v>
+        <v>-14.63556348658886</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>-373.6189085357614</v>
+        <v>-373.6129180285574</v>
       </c>
       <c r="B69" t="n">
-        <v>-14.42266367090804</v>
+        <v>-14.42218040158252</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>-370.9704213535983</v>
+        <v>-370.9646569795685</v>
       </c>
       <c r="B70" t="n">
-        <v>-14.21040041303903</v>
+        <v>-14.20993947358758</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>-368.3126813382383</v>
+        <v>-368.307154618633</v>
       </c>
       <c r="B71" t="n">
-        <v>-13.99929358788981</v>
+        <v>-13.99885555440954</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>-365.6457532115324</v>
+        <v>-365.6404627313224</v>
       </c>
       <c r="B72" t="n">
-        <v>-13.7893560057143</v>
+        <v>-13.78894041755495</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>-362.9697110567643</v>
+        <v>-362.9646410439397</v>
       </c>
       <c r="B73" t="n">
-        <v>-13.58060114012082</v>
+        <v>-13.58020642634227</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>-360.2846101496158</v>
+        <v>-360.2797716173147</v>
       </c>
       <c r="B74" t="n">
-        <v>-13.37304092591475</v>
+        <v>-13.37266761208863</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>-357.5905270863293</v>
+        <v>-357.5859128926795</v>
       </c>
       <c r="B75" t="n">
-        <v>-13.16668888523517</v>
+        <v>-13.16633609069029</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>-354.8875377911669</v>
+        <v>-354.8831560323578</v>
       </c>
       <c r="B76" t="n">
-        <v>-12.96155838946498</v>
+        <v>-12.96122640091295</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>-352.1756880406816</v>
+        <v>-352.1715348921624</v>
       </c>
       <c r="B77" t="n">
-        <v>-12.75766045432735</v>
+        <v>-12.75734865127424</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>-349.4550662725026</v>
+        <v>-349.4511317474088</v>
       </c>
       <c r="B78" t="n">
-        <v>-12.55500924409407</v>
+        <v>-12.55471655830144</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>-346.725729889902</v>
+        <v>-346.7220130370501</v>
       </c>
       <c r="B79" t="n">
-        <v>-12.35361650819092</v>
+        <v>-12.35334255731942</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>-343.9877423655303</v>
+        <v>-343.9842602169075</v>
       </c>
       <c r="B80" t="n">
-        <v>-12.15349438808275</v>
+        <v>-12.15324010142407</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>-341.2411760537325</v>
+        <v>-341.2379157727331</v>
       </c>
       <c r="B81" t="n">
-        <v>-11.95465559849347</v>
+        <v>-11.95441971896247</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>-338.4861093025168</v>
+        <v>-338.4830547944313</v>
       </c>
       <c r="B82" t="n">
-        <v>-11.75711318950343</v>
+        <v>-11.7568942552532</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>-335.7225934097989</v>
+        <v>-335.7197559666628</v>
       </c>
       <c r="B83" t="n">
-        <v>-11.56087818966265</v>
+        <v>-11.56067670891099</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>-332.950703223969</v>
+        <v>-332.9480846806693</v>
       </c>
       <c r="B84" t="n">
-        <v>-11.36596324032399</v>
+        <v>-11.36577903721661</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>-330.170504973489</v>
+        <v>-330.1681071475258</v>
       </c>
       <c r="B85" t="n">
-        <v>-11.17238028448674</v>
+        <v>-11.17221317926919</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>-327.3820615317619</v>
+        <v>-327.3798862233397</v>
       </c>
       <c r="B86" t="n">
-        <v>-10.98014095700756</v>
+        <v>-10.9799907661714</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>-324.5854531104702</v>
+        <v>-324.5834879778962</v>
       </c>
       <c r="B87" t="n">
-        <v>-10.78925800142039</v>
+        <v>-10.78912357803981</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>-321.780737219365</v>
+        <v>-321.7789892566498</v>
       </c>
       <c r="B88" t="n">
-        <v>-10.59974251707084</v>
+        <v>-10.59962404078576</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>-318.9679906373345</v>
+        <v>-318.9664507762616</v>
       </c>
       <c r="B89" t="n">
-        <v>-10.41160683053093</v>
+        <v>-10.41150339842767</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
-        <v>-316.1472731556824</v>
+        <v>-316.1459347166937</v>
       </c>
       <c r="B90" t="n">
-        <v>-10.22486203997514</v>
+        <v>-10.22477292635503</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
-        <v>-313.3186566756283</v>
+        <v>-313.3175411126151</v>
       </c>
       <c r="B91" t="n">
-        <v>-10.0395199707645</v>
+        <v>-10.03944629791528</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
-        <v>-310.4822121613699</v>
+        <v>-310.4812898374654</v>
       </c>
       <c r="B92" t="n">
-        <v>-9.855592290958981</v>
+        <v>-9.855531842781545</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
-        <v>-307.6379993002128</v>
+        <v>-307.6372920508073</v>
       </c>
       <c r="B93" t="n">
-        <v>-9.673089854520896</v>
+        <v>-9.673043761542232</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
-        <v>-304.7861010814561</v>
+        <v>-304.7855965737814</v>
       </c>
       <c r="B94" t="n">
-        <v>-9.492024923259976</v>
+        <v>-9.491992114416007</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
-        <v>-301.9265710980048</v>
+        <v>-301.9262682298449</v>
       </c>
       <c r="B95" t="n">
-        <v>-9.312407794329317</v>
+        <v>-9.312387926221589</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="1" t="n">
-        <v>-299.0594918350333</v>
+        <v>-299.0593834678788</v>
       </c>
       <c r="B96" t="n">
-        <v>-9.134250502397549</v>
+        <v>-9.134242861332183</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
-        <v>-296.18491773498</v>
+        <v>-296.1850203820026</v>
       </c>
       <c r="B97" t="n">
-        <v>-8.957563240602951</v>
+        <v>-8.957568574072582</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="n">
-        <v>-293.302925216938</v>
+        <v>-293.3032201123488</v>
       </c>
       <c r="B98" t="n">
-        <v>-8.782357479434296</v>
+        <v>-8.782374369304478</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
-        <v>-290.413591503346</v>
+        <v>-290.4140890940761</v>
       </c>
       <c r="B99" t="n">
-        <v>-8.608644626332449</v>
+        <v>-8.608673439263953</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
-        <v>-287.5169757972651</v>
+        <v>-287.5176693335586</v>
       </c>
       <c r="B100" t="n">
-        <v>-8.436434909478038</v>
+        <v>-8.43647497538953</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="n">
-        <v>-284.613160473918</v>
+        <v>-284.6140372226678</v>
       </c>
       <c r="B101" t="n">
-        <v>-8.265739846422235</v>
+        <v>-8.265790159354822</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
-        <v>-281.7021884744555</v>
+        <v>-281.7032703667011</v>
       </c>
       <c r="B102" t="n">
-        <v>-8.096568547260944</v>
+        <v>-8.09663013099032</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="n">
-        <v>-278.7841477730352</v>
+        <v>-278.7854335852587</v>
       </c>
       <c r="B103" t="n">
-        <v>-7.928932672446024</v>
+        <v>-7.929005184455036</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
-        <v>-275.8591151749225</v>
+        <v>-275.8605865910004</v>
       </c>
       <c r="B104" t="n">
-        <v>-7.76284310823965</v>
+        <v>-7.762925244040247</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
-        <v>-272.9271508138009</v>
+        <v>-272.9288117756543</v>
       </c>
       <c r="B105" t="n">
-        <v>-7.598309696786629</v>
+        <v>-7.598401430873139</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="n">
-        <v>-269.9883366858234</v>
+        <v>-269.9901748618988</v>
       </c>
       <c r="B106" t="n">
-        <v>-7.435343416108452</v>
+        <v>-7.435443818375433</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="n">
-        <v>-267.0427211132242</v>
+        <v>-267.0447582494876</v>
       </c>
       <c r="B107" t="n">
-        <v>-7.273953281731536</v>
+        <v>-7.274063303360862</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
-        <v>-264.0904039784929</v>
+        <v>-264.0926103014244</v>
       </c>
       <c r="B108" t="n">
-        <v>-7.114151045131933</v>
+        <v>-7.114268822295969</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
-        <v>-261.1314281578338</v>
+        <v>-261.1338194236249</v>
       </c>
       <c r="B109" t="n">
-        <v>-6.95594525161647</v>
+        <v>-6.956071399989042</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
-        <v>-258.1658813246446</v>
+        <v>-258.1684566317879</v>
       </c>
       <c r="B110" t="n">
-        <v>-6.799346773285606</v>
+        <v>-6.799481003133138</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
-        <v>-255.1938357065515</v>
+        <v>-255.1965819322419</v>
       </c>
       <c r="B111" t="n">
-        <v>-6.644365537449232</v>
+        <v>-6.644506928197046</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="1" t="n">
-        <v>-252.2153450847416</v>
+        <v>-252.2182778904401</v>
       </c>
       <c r="B112" t="n">
-        <v>-6.491010424700448</v>
+        <v>-6.491159554795018</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="1" t="n">
-        <v>-249.2304976230438</v>
+        <v>-249.2336105298114</v>
       </c>
       <c r="B113" t="n">
-        <v>-6.339291997572758</v>
+        <v>-6.33944829655843</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
-        <v>-246.2393763400055</v>
+        <v>-246.2426507075173</v>
       </c>
       <c r="B114" t="n">
-        <v>-6.18922041657197</v>
+        <v>-6.189382720827098</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
-        <v>-243.2420245654639</v>
+        <v>-243.2454814958002</v>
       </c>
       <c r="B115" t="n">
-        <v>-6.040803757598326</v>
+        <v>-6.040972895647258</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
-        <v>-240.2385419770698</v>
+        <v>-240.2421635749985</v>
       </c>
       <c r="B116" t="n">
-        <v>-5.894052803576358</v>
+        <v>-5.894227669968217</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="1" t="n">
-        <v>-237.2289830910518</v>
+        <v>-237.2327790037845</v>
       </c>
       <c r="B117" t="n">
-        <v>-5.748975998851222</v>
+        <v>-5.749156842511297</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="1" t="n">
-        <v>-234.2134252808547</v>
+        <v>-234.2173886192221</v>
       </c>
       <c r="B118" t="n">
-        <v>-5.605582809578664</v>
+        <v>-5.605769079843753</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="1" t="n">
-        <v>-231.1919514667755</v>
+        <v>-231.1960753389904</v>
       </c>
       <c r="B119" t="n">
-        <v>-5.463882842653931</v>
+        <v>-5.464074002266045</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
-        <v>-228.1646109354797</v>
+        <v>-228.1689049313135</v>
       </c>
       <c r="B120" t="n">
-        <v>-5.323884027284123</v>
+        <v>-5.324080310116329</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
-        <v>-225.1314981001225</v>
+        <v>-225.1359556525492</v>
       </c>
       <c r="B121" t="n">
-        <v>-5.185596291592503</v>
+        <v>-5.185797181211399</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
-        <v>-222.0926847338356</v>
+        <v>-222.0973040578197</v>
       </c>
       <c r="B122" t="n">
-        <v>-5.049028390473126</v>
+        <v>-5.049233596918043</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
-        <v>-219.0482488663033</v>
+        <v>-219.053017207747</v>
       </c>
       <c r="B123" t="n">
-        <v>-4.914189250210313</v>
+        <v>-4.914398004942427</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="1" t="n">
-        <v>-215.998244955797</v>
+        <v>-216.0031779981518</v>
       </c>
       <c r="B124" t="n">
-        <v>-4.781086655525399</v>
+        <v>-4.781299447260835</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
-        <v>-212.9427628486621</v>
+        <v>-212.9478532963885</v>
       </c>
       <c r="B125" t="n">
-        <v>-4.649729842592109</v>
+        <v>-4.649946149016245</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
-        <v>-209.8818797768167</v>
+        <v>-209.8871148678043</v>
       </c>
       <c r="B126" t="n">
-        <v>-4.520127366379711</v>
+        <v>-4.52034644973466</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
-        <v>-206.8156679257702</v>
+        <v>-206.8210523162889</v>
       </c>
       <c r="B127" t="n">
-        <v>-4.39228745432888</v>
+        <v>-4.392509322648294</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
-        <v>-203.7441835023594</v>
+        <v>-203.7497266213126</v>
       </c>
       <c r="B128" t="n">
-        <v>-4.266217577550918</v>
+        <v>-4.266442424712466</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
-        <v>-200.6675320115318</v>
+        <v>-200.6732152873514</v>
       </c>
       <c r="B129" t="n">
-        <v>-4.141927119627837</v>
+        <v>-4.142153998577811</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="1" t="n">
-        <v>-197.5857637168321</v>
+        <v>-197.5916029841501</v>
       </c>
       <c r="B130" t="n">
-        <v>-4.01942309290925</v>
+        <v>-4.019652449949149</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="1" t="n">
-        <v>-194.4989794359595</v>
+        <v>-194.5049558060952</v>
       </c>
       <c r="B131" t="n">
-        <v>-3.898714422383932</v>
+        <v>-3.89894532604842</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="1" t="n">
-        <v>-191.4072293199507</v>
+        <v>-191.4133470276406</v>
       </c>
       <c r="B132" t="n">
-        <v>-3.779807919715751</v>
+        <v>-3.780040357770247</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
-        <v>-188.3106027927361</v>
+        <v>-188.3168605900732</v>
       </c>
       <c r="B133" t="n">
-        <v>-3.662711820846994</v>
+        <v>-3.662945567117987</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="1" t="n">
-        <v>-185.2091784342015</v>
+        <v>-185.2155689854326</v>
       </c>
       <c r="B134" t="n">
-        <v>-3.547433811334429</v>
+        <v>-3.547668417784536</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
-        <v>-182.1030297628303</v>
+        <v>-182.1095511846597</v>
       </c>
       <c r="B135" t="n">
-        <v>-3.433981270654925</v>
+        <v>-3.434216501051367</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="1" t="n">
-        <v>-178.9922288614686</v>
+        <v>-178.9988856200462</v>
       </c>
       <c r="B136" t="n">
-        <v>-3.322361417540719</v>
+        <v>-3.322597265289517</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
-        <v>-175.8768551927111</v>
+        <v>-175.8836565570712</v>
       </c>
       <c r="B137" t="n">
-        <v>-3.212581622475057</v>
+        <v>-3.212818240115126</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="1" t="n">
-        <v>-172.7569925262934</v>
+        <v>-172.7639093763262</v>
       </c>
       <c r="B138" t="n">
-        <v>-3.104649278478405</v>
+        <v>-3.104885484845454</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="1" t="n">
-        <v>-169.632709302172</v>
+        <v>-169.6397563311421</v>
       </c>
       <c r="B139" t="n">
-        <v>-2.998571126336913</v>
+        <v>-2.998807270285965</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
-        <v>-166.5040897679807</v>
+        <v>-166.5112599039525</v>
       </c>
       <c r="B140" t="n">
-        <v>-2.894354331815038</v>
+        <v>-2.89459001569341</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="1" t="n">
-        <v>-163.3712128245132</v>
+        <v>-163.3785044221037</v>
       </c>
       <c r="B141" t="n">
-        <v>-2.792005749817804</v>
+        <v>-2.792240765237494</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
-        <v>-160.2341520385412</v>
+        <v>-160.2415637277344</v>
       </c>
       <c r="B142" t="n">
-        <v>-2.691531942010727</v>
+        <v>-2.691766092703006</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="1" t="n">
-        <v>-157.0929756547999</v>
+        <v>-157.1005166147034</v>
       </c>
       <c r="B143" t="n">
-        <v>-2.592939194360838</v>
+        <v>-2.593172614637382</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
-        <v>-153.94779111409</v>
+        <v>-153.9554373999102</v>
       </c>
       <c r="B144" t="n">
-        <v>-2.496234889403752</v>
+        <v>-2.496466687523224</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
-        <v>-150.798649431139</v>
+        <v>-150.8064161877569</v>
       </c>
       <c r="B145" t="n">
-        <v>-2.40142453042148</v>
+        <v>-2.401655025690985</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="1" t="n">
-        <v>-147.6456362388753</v>
+        <v>-147.653521759509</v>
       </c>
       <c r="B146" t="n">
-        <v>-2.308514577709957</v>
+        <v>-2.308743569029616</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
-        <v>-144.4888418219402</v>
+        <v>-144.4968275960122</v>
       </c>
       <c r="B147" t="n">
-        <v>-2.217511482693027</v>
+        <v>-2.217738293017675</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="1" t="n">
-        <v>-141.3283348823309</v>
+        <v>-141.3364305742743</v>
       </c>
       <c r="B148" t="n">
-        <v>-2.128420941446848</v>
+        <v>-2.128645714717095</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="1" t="n">
-        <v>-138.1642007349489</v>
+        <v>-138.1723992008402</v>
       </c>
       <c r="B149" t="n">
-        <v>-2.041249004448986</v>
+        <v>-2.041471408277602</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="1" t="n">
-        <v>-134.9965025971995</v>
+        <v>-135.0048183303786</v>
       </c>
       <c r="B150" t="n">
-        <v>-1.956000993304826</v>
+        <v>-1.956221284731328</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="1" t="n">
-        <v>-131.8253535333198</v>
+        <v>-131.83375721047</v>
       </c>
       <c r="B151" t="n">
-        <v>-1.872683439914397</v>
+        <v>-1.872900710326746</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="1" t="n">
-        <v>-128.6508061120787</v>
+        <v>-128.6593016616121</v>
       </c>
       <c r="B152" t="n">
-        <v>-1.791301131674061</v>
+        <v>-1.791515371013162</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="1" t="n">
-        <v>-125.4729511277737</v>
+        <v>-125.4815424550374</v>
       </c>
       <c r="B153" t="n">
-        <v>-1.711859742828807</v>
+        <v>-1.712070932703426</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="1" t="n">
-        <v>-122.2918634939859</v>
+        <v>-122.3005542282172</v>
       </c>
       <c r="B154" t="n">
-        <v>-1.634364410411962</v>
+        <v>-1.634572518511874</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="1" t="n">
-        <v>-119.1076177033884</v>
+        <v>-119.1164060595936</v>
       </c>
       <c r="B155" t="n">
-        <v>-1.55882014723403</v>
+        <v>-1.559025007638638</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="1" t="n">
-        <v>-115.9203109471446</v>
+        <v>-115.9291840836481</v>
       </c>
       <c r="B156" t="n">
-        <v>-1.485232369817226</v>
+        <v>-1.485433567981147</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="1" t="n">
-        <v>-112.7300235161008</v>
+        <v>-112.7389850393786</v>
       </c>
       <c r="B157" t="n">
-        <v>-1.413605949061804</v>
+        <v>-1.413803459004072</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="1" t="n">
-        <v>-109.5368245007582</v>
+        <v>-109.5458674599286</v>
       </c>
       <c r="B158" t="n">
-        <v>-1.343945386499087</v>
+        <v>-1.34413894861359</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="1" t="n">
-        <v>-106.3408005048322</v>
+        <v>-106.3499282390868</v>
       </c>
       <c r="B159" t="n">
-        <v>-1.276255449512462</v>
+        <v>-1.276445032044251</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="1" t="n">
-        <v>-103.142031577803</v>
+        <v>-103.1512427539577</v>
       </c>
       <c r="B160" t="n">
-        <v>-1.210540628371746</v>
+        <v>-1.210726098685853</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="1" t="n">
-        <v>-99.94060469410563</v>
+        <v>-99.94989136854019</v>
       </c>
       <c r="B161" t="n">
-        <v>-1.14680542135099</v>
+        <v>-1.14698651970815</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="1" t="n">
-        <v>-96.73660004929748</v>
+        <v>-96.74595524573519</v>
       </c>
       <c r="B162" t="n">
-        <v>-1.085054052631961</v>
+        <v>-1.08523055278647</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="1" t="n">
-        <v>-93.5300984016724</v>
+        <v>-93.53952591090258</v>
       </c>
       <c r="B163" t="n">
-        <v>-1.025290628474238</v>
+        <v>-1.025462514763774</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="1" t="n">
-        <v>-90.32116442197903</v>
+        <v>-90.3306734055017</v>
       </c>
       <c r="B164" t="n">
-        <v>-0.9675188406175721</v>
+        <v>-0.9676861854384811</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="1" t="n">
-        <v>-87.10991203455781</v>
+        <v>-87.11948939389166</v>
       </c>
       <c r="B165" t="n">
-        <v>-0.9117431327728696</v>
+        <v>-0.9119056108342534</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="1" t="n">
-        <v>-83.89640579919909</v>
+        <v>-83.90604429450177</v>
       </c>
       <c r="B166" t="n">
-        <v>-0.8579669232404399</v>
+        <v>-0.8581243307010311</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="1" t="n">
-        <v>-80.6807321264113</v>
+        <v>-80.69043012719757</v>
       </c>
       <c r="B167" t="n">
-        <v>-0.8061938870019674</v>
+        <v>-0.806346122220333</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="1" t="n">
-        <v>-77.46296672332174</v>
+        <v>-77.47273335161529</v>
       </c>
       <c r="B168" t="n">
-        <v>-0.7564273925291616</v>
+        <v>-0.7565745199581784</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="1" t="n">
-        <v>-74.24320218522362</v>
+        <v>-74.25302411862549</v>
       </c>
       <c r="B169" t="n">
-        <v>-0.7086709367409867</v>
+        <v>-0.7088126774384023</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="1" t="n">
-        <v>-71.02151365403114</v>
+        <v>-71.03138946779978</v>
       </c>
       <c r="B170" t="n">
-        <v>-0.6629276140602656</v>
+        <v>-0.6630638797000188</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="1" t="n">
-        <v>-67.79799382813553</v>
+        <v>-67.80792701483203</v>
       </c>
       <c r="B171" t="n">
-        <v>-0.6192006362325628</v>
+        <v>-0.6193314061202102</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="1" t="n">
-        <v>-64.57271303910613</v>
+        <v>-64.58269632875601</v>
       </c>
       <c r="B172" t="n">
-        <v>-0.5774927722343648</v>
+        <v>-0.5776178834416896</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="1" t="n">
-        <v>-61.34576923160873</v>
+        <v>-61.35579513112401</v>
       </c>
       <c r="B173" t="n">
-        <v>-0.537807018976622</v>
+        <v>-0.5379263193771351</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="1" t="n">
-        <v>-58.11722702874166</v>
+        <v>-58.12729945723294</v>
       </c>
       <c r="B174" t="n">
-        <v>-0.5001458210287524</v>
+        <v>-0.5002593025870681</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="1" t="n">
-        <v>-54.88717953152653</v>
+        <v>-54.89730711333954</v>
       </c>
       <c r="B175" t="n">
-        <v>-0.4645118396646239</v>
+        <v>-0.4646195370716271</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="1" t="n">
-        <v>-51.65571340212911</v>
+        <v>-51.66588347739155</v>
       </c>
       <c r="B176" t="n">
-        <v>-0.4309075098392441</v>
+        <v>-0.4310092266723871</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="1" t="n">
-        <v>-48.42291578159255</v>
+        <v>-48.43311547483003</v>
       </c>
       <c r="B177" t="n">
-        <v>-0.3993351261464397</v>
+        <v>-0.3994306878458644</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="1" t="n">
-        <v>-45.18886288579929</v>
+        <v>-45.1990956583507</v>
       </c>
       <c r="B178" t="n">
-        <v>-0.3697967404586393</v>
+        <v>-0.3698861410641143</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="1" t="n">
-        <v>-41.95363075890409</v>
+        <v>-41.9639058674862</v>
       </c>
       <c r="B179" t="n">
-        <v>-0.3422942847170134</v>
+        <v>-0.3423775592333982</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="1" t="n">
-        <v>-38.71731782843555</v>
+        <v>-38.72762217724998</v>
       </c>
       <c r="B180" t="n">
-        <v>-0.3168297422608077</v>
+        <v>-0.3169067389530653</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="1" t="n">
-        <v>-35.47999999152064</v>
+        <v>-35.49033187063916</v>
       </c>
       <c r="B181" t="n">
-        <v>-0.293404765358332</v>
+        <v>-0.2934754362095759</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="1" t="n">
-        <v>-32.24176477528384</v>
+        <v>-32.25212762785644</v>
       </c>
       <c r="B182" t="n">
-        <v>-0.2720209618460956</v>
+        <v>-0.2720852943777174</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="1" t="n">
-        <v>-29.00269951719753</v>
+        <v>-29.01307509127257</v>
       </c>
       <c r="B183" t="n">
-        <v>-0.2526797913228904</v>
+        <v>-0.2527376436616464</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="1" t="n">
-        <v>-25.76288020559103</v>
+        <v>-25.77328310259912</v>
       </c>
       <c r="B184" t="n">
-        <v>-0.2353825094181161</v>
+        <v>-0.2354339394960618</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="1" t="n">
-        <v>-22.52239464988883</v>
+        <v>-22.5328117746925</v>
       </c>
       <c r="B185" t="n">
-        <v>-0.2201303059215149</v>
+        <v>-0.2201752221660627</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="1" t="n">
-        <v>-19.28132425438637</v>
+        <v>-19.29176483067081</v>
       </c>
       <c r="B186" t="n">
-        <v>-0.2069241984826533</v>
+        <v>-0.2069626180762612</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="1" t="n">
-        <v>-16.03975665294326</v>
+        <v>-16.0502022168778</v>
       </c>
       <c r="B187" t="n">
-        <v>-0.1957650926262033</v>
+        <v>-0.1957969285159606</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="1" t="n">
-        <v>-12.79777370422316</v>
+        <v>-12.80822768719755</v>
       </c>
       <c r="B188" t="n">
-        <v>-0.1866537318783799</v>
+        <v>-0.186678986657796</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="1" t="n">
-        <v>-9.555462648528653</v>
+        <v>-9.565934266600436</v>
       </c>
       <c r="B189" t="n">
-        <v>-0.1795907370114662</v>
+        <v>-0.1796094174285372</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="1" t="n">
-        <v>-6.312900208843121</v>
+        <v>-6.323376575789477</v>
       </c>
       <c r="B190" t="n">
-        <v>-0.1745765691465522</v>
+        <v>-0.1745886373076644</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="1" t="n">
-        <v>-3.070179010875414</v>
+        <v>-3.080658186022802</v>
       </c>
       <c r="B191" t="n">
-        <v>-0.1716115793373945</v>
+        <v>-0.1716170281304414</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="1" t="n">
-        <v>0.1726244192368247</v>
+        <v>0.1621387999721795</v>
       </c>
       <c r="B192" t="n">
-        <v>-0.1706959587311303</v>
+        <v>-0.1706947846257378</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="1" t="n">
-        <v>3.415411663158736</v>
+        <v>3.404932694777011</v>
       </c>
       <c r="B193" t="n">
-        <v>-0.1718297649463238</v>
+        <v>-0.1718219682852009</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="1" t="n">
-        <v>6.658117346879786</v>
+        <v>6.64764139343102</v>
       </c>
       <c r="B194" t="n">
-        <v>-0.175012923027424</v>
+        <v>-0.1749985075959728</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="1" t="n">
-        <v>9.90064284615241</v>
+        <v>9.890166270743846</v>
       </c>
       <c r="B195" t="n">
-        <v>-0.1802452033333566</v>
+        <v>-0.1802241656823753</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="n">
-        <v>13.14290648217114</v>
+        <v>13.13243680176767</v>
       </c>
       <c r="B196" t="n">
-        <v>-0.1875262440039194</v>
+        <v>-0.1874986023134113</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="1" t="n">
-        <v>16.38483174432102</v>
+        <v>16.37437626644921</v>
       </c>
       <c r="B197" t="n">
-        <v>-0.196855567121446</v>
+        <v>-0.1968213532459231</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="1" t="n">
-        <v>19.62632581795809</v>
+        <v>19.61588648083842</v>
       </c>
       <c r="B198" t="n">
-        <v>-0.2082325133874576</v>
+        <v>-0.2081917522668846</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="1" t="n">
-        <v>22.86731200655376</v>
+        <v>22.85689095781071</v>
       </c>
       <c r="B199" t="n">
-        <v>-0.2216563344108522</v>
+        <v>-0.2216090556815118</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="1" t="n">
-        <v>26.10769236313056</v>
+        <v>26.09729111690158</v>
       </c>
       <c r="B200" t="n">
-        <v>-0.2371260542738014</v>
+        <v>-0.2370722880839082</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="1" t="n">
-        <v>29.34740675661478</v>
+        <v>29.33702208733256</v>
       </c>
       <c r="B201" t="n">
-        <v>-0.254640739091144</v>
+        <v>-0.2545804917384089</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="1" t="n">
-        <v>32.58634053499418</v>
+        <v>32.57598511398317</v>
       </c>
       <c r="B202" t="n">
-        <v>-0.2741990317437057</v>
+        <v>-0.2741324037486379</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="n">
-        <v>35.82443382581928</v>
+        <v>35.8141095834069</v>
       </c>
       <c r="B203" t="n">
-        <v>-0.2957997409030781</v>
+        <v>-0.2957267821927871</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="n">
-        <v>39.06159371452812</v>
+        <v>39.05130279237452</v>
       </c>
       <c r="B204" t="n">
-        <v>-0.3194413469250321</v>
+        <v>-0.3193621124753179</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="n">
-        <v>42.29774406633911</v>
+        <v>42.28747721807694</v>
       </c>
       <c r="B205" t="n">
-        <v>-0.3451223074991105</v>
+        <v>-0.3450367624632236</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="n">
-        <v>45.53279223664642</v>
+        <v>45.52255116469627</v>
       </c>
       <c r="B206" t="n">
-        <v>-0.3728408155805596</v>
+        <v>-0.3727490046171908</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="n">
-        <v>48.7666507646181</v>
+        <v>48.75644877760389</v>
       </c>
       <c r="B207" t="n">
-        <v>-0.4025949532714321</v>
+        <v>-0.4024970345666645</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="n">
-        <v>51.99924383484117</v>
+        <v>51.98908800680759</v>
       </c>
       <c r="B208" t="n">
-        <v>-0.434382773652203</v>
+        <v>-0.4342788674571807</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="n">
-        <v>55.23048405955573</v>
+        <v>55.22036555414184</v>
       </c>
       <c r="B209" t="n">
-        <v>-0.4682020877254729</v>
+        <v>-0.4680921560841114</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="n">
-        <v>58.46029549295852</v>
+        <v>58.45021599682435</v>
       </c>
       <c r="B210" t="n">
-        <v>-0.5040506901052311</v>
+        <v>-0.5039347984843232</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="n">
-        <v>61.68858545058891</v>
+        <v>61.67855783752847</v>
       </c>
       <c r="B211" t="n">
-        <v>-0.5419260563030832</v>
+        <v>-0.5418044078922719</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="n">
-        <v>64.91526710129963</v>
+        <v>64.90529887212591</v>
       </c>
       <c r="B212" t="n">
-        <v>-0.5818255757442046</v>
+        <v>-0.5816983299453682</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="n">
-        <v>68.14028099928345</v>
+        <v>68.13035187082468</v>
       </c>
       <c r="B213" t="n">
-        <v>-0.6237468565809365</v>
+        <v>-0.6236138175675308</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="n">
-        <v>71.36351240950681</v>
+        <v>71.3536410755422</v>
       </c>
       <c r="B214" t="n">
-        <v>-0.6676866610234811</v>
+        <v>-0.6675481373496837</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="n">
-        <v>74.58489683528974</v>
+        <v>74.57508495918665</v>
       </c>
       <c r="B215" t="n">
-        <v>-0.7136422667572333</v>
+        <v>-0.713498354524944</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="n">
-        <v>77.8043474289781</v>
+        <v>77.79459689246265</v>
       </c>
       <c r="B216" t="n">
-        <v>-0.7616105231926724</v>
+        <v>-0.7614613248607895</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="n">
-        <v>81.02178838722844</v>
+        <v>81.01209007147085</v>
       </c>
       <c r="B217" t="n">
-        <v>-0.8115883092410172</v>
+        <v>-0.8114337566029803</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="n">
-        <v>84.2371165914775</v>
+        <v>84.22749412617605</v>
       </c>
       <c r="B218" t="n">
-        <v>-0.8635719368423906</v>
+        <v>-0.8634124836881369</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="n">
-        <v>87.45027273423894</v>
+        <v>87.44071160040333</v>
       </c>
       <c r="B219" t="n">
-        <v>-0.9175582804590476</v>
+        <v>-0.9173937729489978</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="n">
-        <v>90.66115919152863</v>
+        <v>90.65166686290817</v>
       </c>
       <c r="B220" t="n">
-        <v>-0.9735434597093615</v>
+        <v>-0.9733741064718231</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="n">
-        <v>93.86970063842406</v>
+        <v>93.86027896720056</v>
       </c>
       <c r="B221" t="n">
-        <v>-1.031523831244868</v>
+        <v>-1.031349751849007</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="n">
-        <v>97.07581620479144</v>
+        <v>97.06646117034272</v>
       </c>
       <c r="B222" t="n">
-        <v>-1.091495530343423</v>
+        <v>-1.091316736190748</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="n">
-        <v>100.2794192210509</v>
+        <v>100.2701385231302</v>
       </c>
       <c r="B223" t="n">
-        <v>-1.153454448407075</v>
+        <v>-1.153271173502418</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="n">
-        <v>103.4804291893521</v>
+        <v>103.4712300518529</v>
       </c>
       <c r="B224" t="n">
-        <v>-1.217396457262367</v>
+        <v>-1.217208940607151</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="n">
-        <v>106.6787652061484</v>
+        <v>106.6696438182927</v>
       </c>
       <c r="B225" t="n">
-        <v>-1.283317291217855</v>
+        <v>-1.283125554666157</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="n">
-        <v>109.8743520786866</v>
+        <v>109.8653102535903</v>
       </c>
       <c r="B226" t="n">
-        <v>-1.351212677634805</v>
+        <v>-1.351016857126268</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="n">
-        <v>113.0670869690388</v>
+        <v>113.0581378027537</v>
       </c>
       <c r="B227" t="n">
-        <v>-1.421077615236612</v>
+        <v>-1.420878100224542</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="n">
-        <v>116.2569063622722</v>
+        <v>116.2480460176158</v>
       </c>
       <c r="B228" t="n">
-        <v>-1.492907814199924</v>
+        <v>-1.492704632783756</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="n">
-        <v>119.4437294049244</v>
+        <v>119.4349650796665</v>
       </c>
       <c r="B229" t="n">
-        <v>-1.566698492382102</v>
+        <v>-1.566491924367995</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="n">
-        <v>122.627476075345</v>
+        <v>122.6187928440397</v>
       </c>
       <c r="B230" t="n">
-        <v>-1.642444758004302</v>
+        <v>-1.642234563566831</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="n">
-        <v>125.8080602686188</v>
+        <v>125.7994709611893</v>
       </c>
       <c r="B231" t="n">
-        <v>-1.720141441239292</v>
+        <v>-1.71992803874997</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="n">
-        <v>128.9853961997616</v>
+        <v>128.9769025829471</v>
       </c>
       <c r="B232" t="n">
-        <v>-1.799783237309811</v>
+        <v>-1.799566788767493</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="n">
-        <v>132.1594149016205</v>
+        <v>132.1510135880785</v>
       </c>
       <c r="B233" t="n">
-        <v>-1.881365136523243</v>
+        <v>-1.881145673420008</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="n">
-        <v>135.330025351238</v>
+        <v>135.3217232357661</v>
       </c>
       <c r="B234" t="n">
-        <v>-1.964881442380403</v>
+        <v>-1.964659263615886</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="n">
-        <v>138.4971530917165</v>
+        <v>138.4889630056848</v>
       </c>
       <c r="B235" t="n">
-        <v>-2.050326754735806</v>
+        <v>-2.050102334573324</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="n">
-        <v>141.6607123961695</v>
+        <v>141.6526360831735</v>
       </c>
       <c r="B236" t="n">
-        <v>-2.137695245648672</v>
+        <v>-2.137468773101489</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="n">
-        <v>144.820640354314</v>
+        <v>144.8126687166878</v>
       </c>
       <c r="B237" t="n">
-        <v>-2.226981596742377</v>
+        <v>-2.226752954776032</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="n">
-        <v>147.9768462771784</v>
+        <v>147.9689804807463</v>
       </c>
       <c r="B238" t="n">
-        <v>-2.318179595213422</v>
+        <v>-2.31794894893298</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="n">
-        <v>151.1292444045843</v>
+        <v>151.1214921216741</v>
       </c>
       <c r="B239" t="n">
-        <v>-2.411283020672641</v>
+        <v>-2.411050731610032</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="n">
-        <v>154.2777669804787</v>
+        <v>154.2701296314933</v>
       </c>
       <c r="B240" t="n">
-        <v>-2.506286059535967</v>
+        <v>-2.50605231356522</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="n">
-        <v>157.4223284166665</v>
+        <v>157.4148022616484</v>
       </c>
       <c r="B241" t="n">
-        <v>-2.603182247663483</v>
+        <v>-2.602947072631878</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="n">
-        <v>160.5628497490364</v>
+        <v>160.5554475998287</v>
       </c>
       <c r="B242" t="n">
-        <v>-2.701965189895162</v>
+        <v>-2.701729132404751</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="n">
-        <v>163.6992515400972</v>
+        <v>163.6919750715018</v>
       </c>
       <c r="B243" t="n">
-        <v>-2.802628351394532</v>
+        <v>-2.802391621716055</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="n">
-        <v>166.8314655917337</v>
+        <v>166.8242995868939</v>
       </c>
       <c r="B244" t="n">
-        <v>-2.905165443081074</v>
+        <v>-2.904927696662156</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="n">
-        <v>169.9593960560591</v>
+        <v>169.9523756377142</v>
       </c>
       <c r="B245" t="n">
-        <v>-3.00956914821171</v>
+        <v>-3.009331707188494</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="n">
-        <v>173.0829918163692</v>
+        <v>173.0760908652595</v>
       </c>
       <c r="B246" t="n">
-        <v>-3.115833517686212</v>
+        <v>-3.115595669389279</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="n">
-        <v>176.202157502594</v>
+        <v>176.1953773338094</v>
       </c>
       <c r="B247" t="n">
-        <v>-3.223951002559204</v>
+        <v>-3.223712943503102</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="n">
-        <v>179.3168080734908</v>
+        <v>179.3101617788743</v>
       </c>
       <c r="B248" t="n">
-        <v>-3.333914255539781</v>
+        <v>-3.333676604245397</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="n">
-        <v>182.4268818502251</v>
+        <v>182.4203652876251</v>
       </c>
       <c r="B249" t="n">
-        <v>-3.445716636594938</v>
+        <v>-3.445479412183033</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="n">
-        <v>185.5322891330504</v>
+        <v>185.5259150960957</v>
       </c>
       <c r="B250" t="n">
-        <v>-3.559350392536373</v>
+        <v>-3.55911423110814</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="n">
-        <v>188.6329678489116</v>
+        <v>188.6267209508647</v>
       </c>
       <c r="B251" t="n">
-        <v>-3.674808655689333</v>
+        <v>-3.674573160123145</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="n">
-        <v>191.7288284647445</v>
+        <v>191.7227269364649</v>
       </c>
       <c r="B252" t="n">
-        <v>-3.792083429760481</v>
+        <v>-3.791849457273514</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="n">
-        <v>194.8198033312801</v>
+        <v>194.8138378216867</v>
       </c>
       <c r="B253" t="n">
-        <v>-3.911167417141229</v>
+        <v>-3.910934789087662</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="n">
-        <v>197.9058030605296</v>
+        <v>197.8999863518384</v>
       </c>
       <c r="B254" t="n">
-        <v>-4.032052367804994</v>
+        <v>-4.031821761414676</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="n">
-        <v>200.986766607871</v>
+        <v>200.9810944578619</v>
       </c>
       <c r="B255" t="n">
-        <v>-4.154731018465782</v>
+        <v>-4.154502452765769</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="n">
-        <v>204.0626150384</v>
+        <v>204.0570892974833</v>
       </c>
       <c r="B256" t="n">
-        <v>-4.279195299259641</v>
+        <v>-4.278969033742328</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="n">
-        <v>207.1332711236202</v>
+        <v>207.1278926451112</v>
       </c>
       <c r="B257" t="n">
-        <v>-4.40543708791364</v>
+        <v>-4.405213344411663</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="n">
-        <v>210.1986560728325</v>
+        <v>210.1934266821121</v>
       </c>
       <c r="B258" t="n">
-        <v>-4.533448077626247</v>
+        <v>-4.533227120647553</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="n">
-        <v>213.2586979680641</v>
+        <v>213.2536304406424</v>
       </c>
       <c r="B259" t="n">
-        <v>-4.66322013242484</v>
+        <v>-4.663002698213319</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="n">
-        <v>216.3133297967842</v>
+        <v>216.3084143254626</v>
       </c>
       <c r="B260" t="n">
-        <v>-4.79474522433074</v>
+        <v>-4.79453109465581</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="n">
-        <v>219.362451745146</v>
+        <v>219.357706582019</v>
       </c>
       <c r="B261" t="n">
-        <v>-4.928013789802264</v>
+        <v>-4.927803962517174</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="n">
-        <v>222.4060195661466</v>
+        <v>222.4014293796985</v>
       </c>
       <c r="B262" t="n">
-        <v>-5.063018569883582</v>
+        <v>-5.062812578746019</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="n">
-        <v>225.4439500566386</v>
+        <v>225.4395159321172</v>
       </c>
       <c r="B263" t="n">
-        <v>-5.199750508071787</v>
+        <v>-5.199548601163059</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="n">
-        <v>228.4761600614436</v>
+        <v>228.4718837673471</v>
       </c>
       <c r="B264" t="n">
-        <v>-5.338200416463366</v>
+        <v>-5.338002875390487</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="n">
-        <v>231.5025771072486</v>
+        <v>231.4984659070298</v>
       </c>
       <c r="B265" t="n">
-        <v>-5.478359471532656</v>
+        <v>-5.478166837964238</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="n">
-        <v>234.5231415798937</v>
+        <v>234.5191906639038</v>
       </c>
       <c r="B266" t="n">
-        <v>-5.620219352209944</v>
+        <v>-5.620031611622494</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="n">
-        <v>237.5377643147674</v>
+        <v>237.5339864325836</v>
       </c>
       <c r="B267" t="n">
-        <v>-5.763770249532115</v>
+        <v>-5.763588219783969</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="n">
-        <v>240.5463792746585</v>
+        <v>240.5427706694153</v>
       </c>
       <c r="B268" t="n">
-        <v>-5.90900332918838</v>
+        <v>-5.908827051402113</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="n">
-        <v>243.5489150021525</v>
+        <v>243.5454766767629</v>
       </c>
       <c r="B269" t="n">
-        <v>-6.055909401842058</v>
+        <v>-6.055739144528076</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="n">
-        <v>246.5452942253401</v>
+        <v>246.5420330488399</v>
       </c>
       <c r="B270" t="n">
-        <v>-6.2044788858706</v>
+        <v>-6.204315212506856</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="n">
-        <v>249.5354511303664</v>
+        <v>249.5323684509479</v>
       </c>
       <c r="B271" t="n">
-        <v>-6.35470266146973</v>
+        <v>-6.354545870393196</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="n">
-        <v>252.5193085606271</v>
+        <v>252.5163942853127</v>
       </c>
       <c r="B272" t="n">
-        <v>-6.506570941111676</v>
+        <v>-6.506420747418929</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="n">
-        <v>255.4967949236708</v>
+        <v>255.4940621730374</v>
       </c>
       <c r="B273" t="n">
-        <v>-6.660074108956252</v>
+        <v>-6.659931412700359</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="n">
-        <v>258.4678449780558</v>
+        <v>258.4652887660231</v>
       </c>
       <c r="B274" t="n">
-        <v>-6.815202781045201</v>
+        <v>-6.815067557274631</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="n">
-        <v>261.432369871483</v>
+        <v>261.4299977916849</v>
       </c>
       <c r="B275" t="n">
-        <v>-6.971946232787076</v>
+        <v>-6.971819115961409</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="n">
-        <v>264.3903159177707</v>
+        <v>264.3881173961906</v>
       </c>
       <c r="B276" t="n">
-        <v>-7.130295485834978</v>
+        <v>-7.130176147739178</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="n">
-        <v>267.3416002550832</v>
+        <v>267.3395995102687</v>
       </c>
       <c r="B277" t="n">
-        <v>-7.29023991780582</v>
+        <v>-7.290129906457878</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="n">
-        <v>270.2861689477417</v>
+        <v>270.2843442681515</v>
       </c>
       <c r="B278" t="n">
-        <v>-7.451770371089481</v>
+        <v>-7.451668748671949</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="n">
-        <v>273.2239332434033</v>
+        <v>273.222291805249</v>
       </c>
       <c r="B279" t="n">
-        <v>-7.614875690311578</v>
+        <v>-7.61478308926894</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="n">
-        <v>276.154828587243</v>
+        <v>276.1533827332928</v>
       </c>
       <c r="B280" t="n">
-        <v>-7.779545940809072</v>
+        <v>-7.779463300544307</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="n">
-        <v>279.0787829072635</v>
+        <v>279.0775227392694</v>
       </c>
       <c r="B281" t="n">
-        <v>-7.945770676642752</v>
+        <v>-7.945697689822424</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="n">
-        <v>281.9957317365922</v>
+        <v>281.9946640224617</v>
       </c>
       <c r="B282" t="n">
-        <v>-8.113539790110792</v>
+        <v>-8.113477094431687</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="n">
-        <v>284.9055918987527</v>
+        <v>284.9047293917728</v>
       </c>
       <c r="B283" t="n">
-        <v>-8.282841998269703</v>
+        <v>-8.282790595441384</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="n">
-        <v>287.8083161147878</v>
+        <v>287.8076364689289</v>
       </c>
       <c r="B284" t="n">
-        <v>-8.453668011380017</v>
+        <v>-8.453626852365915</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="n">
-        <v>290.7038092352855</v>
+        <v>290.7033315901436</v>
       </c>
       <c r="B285" t="n">
-        <v>-8.626005641038006</v>
+        <v>-8.625976115158664</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="n">
-        <v>293.5920120286447</v>
+        <v>293.5917427282365</v>
       </c>
       <c r="B286" t="n">
-        <v>-8.799844709932756</v>
+        <v>-8.799827471275762</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="n">
-        <v>296.4728713317533</v>
+        <v>296.4727827333097</v>
       </c>
       <c r="B287" t="n">
-        <v>-8.975175346152952</v>
+        <v>-8.97516898278846</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="n">
-        <v>299.3462979262456</v>
+        <v>299.3464091929567</v>
       </c>
       <c r="B288" t="n">
-        <v>-9.151985399068508</v>
+        <v>-9.151991339311451</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="n">
-        <v>302.2122214277216</v>
+        <v>302.2125388641067</v>
       </c>
       <c r="B289" t="n">
-        <v>-9.330263749853259</v>
+        <v>-9.330282657163963</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="n">
-        <v>305.0705822341291</v>
+        <v>305.0711069627077</v>
       </c>
       <c r="B290" t="n">
-        <v>-9.509999866427421</v>
+        <v>-9.51003209039331</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="n">
-        <v>307.9213030597575</v>
+        <v>307.922041805776</v>
       </c>
       <c r="B291" t="n">
-        <v>-9.69118202217993</v>
+        <v>-9.691228273140467</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="n">
-        <v>310.7643242774222</v>
+        <v>310.7652669118792</v>
       </c>
       <c r="B292" t="n">
-        <v>-9.87379951768483</v>
+        <v>-9.873859432317545</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="n">
-        <v>313.5995810821393</v>
+        <v>313.6007282476484</v>
       </c>
       <c r="B293" t="n">
-        <v>-10.05784125139124</v>
+        <v>-10.05791514955132</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="n">
-        <v>316.4269956439912</v>
+        <v>316.4283544733159</v>
       </c>
       <c r="B294" t="n">
-        <v>-10.24329518542547</v>
+        <v>-10.24338381673675</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="n">
-        <v>319.2464969959914</v>
+        <v>319.2480568410749</v>
       </c>
       <c r="B295" t="n">
-        <v>-10.43014962587876</v>
+        <v>-10.43025257089835</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="n">
-        <v>322.0580314854702</v>
+        <v>322.0598051068358</v>
       </c>
       <c r="B296" t="n">
-        <v>-10.61839394971142</v>
+        <v>-10.6185123437383</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="n">
-        <v>324.8615037164732</v>
+        <v>324.8634982526433</v>
       </c>
       <c r="B297" t="n">
-        <v>-10.80801465095831</v>
+        <v>-10.80814927358824</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="n">
-        <v>327.6568721100469</v>
+        <v>327.6590735852207</v>
       </c>
       <c r="B298" t="n">
-        <v>-10.99900175805945</v>
+        <v>-10.99915195517309</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="n">
-        <v>330.4440678885829</v>
+        <v>330.4464801409294</v>
       </c>
       <c r="B299" t="n">
-        <v>-11.1913434015766</v>
+        <v>-11.19150972684236</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="n">
-        <v>333.2229953460098</v>
+        <v>333.2256316102565</v>
       </c>
       <c r="B300" t="n">
-        <v>-11.38502574095793</v>
+        <v>-11.38520941427814</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="n">
-        <v>335.9936127723325</v>
+        <v>335.9964707867462</v>
       </c>
       <c r="B301" t="n">
-        <v>-11.58003859356722</v>
+        <v>-11.58023976793282</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="n">
-        <v>338.7558686225206</v>
+        <v>338.7589257725257</v>
       </c>
       <c r="B302" t="n">
-        <v>-11.77637106438422</v>
+        <v>-11.77658843598419</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="n">
-        <v>341.5096436761913</v>
+        <v>341.5129330841825</v>
       </c>
       <c r="B303" t="n">
-        <v>-11.97400734325214</v>
+        <v>-11.97424358048488</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="n">
-        <v>344.2549073865875</v>
+        <v>344.2584219814806</v>
       </c>
       <c r="B304" t="n">
-        <v>-12.17293785009576</v>
+        <v>-12.17319276608222</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="n">
-        <v>346.991587101889</v>
+        <v>346.9953184078549</v>
       </c>
       <c r="B305" t="n">
-        <v>-12.3731499343736</v>
+        <v>-12.37342322510813</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="n">
-        <v>349.7196142534867</v>
+        <v>349.723566078661</v>
       </c>
       <c r="B306" t="n">
-        <v>-12.57463115479791</v>
+        <v>-12.57492341149455</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="n">
-        <v>352.4389121337685</v>
+        <v>352.4430887492692</v>
       </c>
       <c r="B307" t="n">
-        <v>-12.77736837969096</v>
+        <v>-12.77768023718664</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="n">
-        <v>355.1494270926013</v>
+        <v>355.1538265970422</v>
       </c>
       <c r="B308" t="n">
-        <v>-12.98135011660534</v>
+        <v>-12.98168175380113</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="n">
-        <v>357.8510801970496</v>
+        <v>357.8557116656273</v>
       </c>
       <c r="B309" t="n">
-        <v>-13.18656290666621</v>
+        <v>-13.18691533710347</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="n">
-        <v>360.5438066382729</v>
+        <v>360.5486628908087</v>
       </c>
       <c r="B310" t="n">
-        <v>-13.39299427026265</v>
+        <v>-13.39336727615611</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="n">
-        <v>363.2275428496633</v>
+        <v>363.2326305648619</v>
       </c>
       <c r="B311" t="n">
-        <v>-13.60063175638052</v>
+        <v>-13.60102618373134</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="n">
-        <v>365.9022246532524</v>
+        <v>365.907541440833</v>
       </c>
       <c r="B312" t="n">
-        <v>-13.80946280333541</v>
+        <v>-13.80987880244433</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="n">
-        <v>368.567762831468</v>
+        <v>368.5733191867066</v>
       </c>
       <c r="B313" t="n">
-        <v>-14.01947280419165</v>
+        <v>-14.01991154113011</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="n">
-        <v>371.2241263379426</v>
+        <v>371.2299049985633</v>
       </c>
       <c r="B314" t="n">
-        <v>-14.2306516613732</v>
+        <v>-14.2311121107862</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="n">
-        <v>373.8712169187363</v>
+        <v>373.8772274506714</v>
       </c>
       <c r="B315" t="n">
-        <v>-14.4429838968008</v>
+        <v>-14.44346715879169</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="1" t="n">
-        <v>376.5089724900613</v>
+        <v>376.5152191766381</v>
       </c>
       <c r="B316" t="n">
-        <v>-14.65645681327868</v>
+        <v>-14.65696358085853</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="1" t="n">
-        <v>379.137336572072</v>
+        <v>379.143820353212</v>
       </c>
       <c r="B317" t="n">
-        <v>-14.87105811881321</v>
+        <v>-14.87158882233672</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="n">
-        <v>381.7562409308688</v>
+        <v>381.7629531241572</v>
       </c>
       <c r="B318" t="n">
-        <v>-15.08677451298539</v>
+        <v>-15.08732879060398</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="n">
-        <v>384.3656011949115</v>
+        <v>384.3725586182796</v>
       </c>
       <c r="B319" t="n">
-        <v>-15.30359127979182</v>
+        <v>-15.30417088051348</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="1" t="n">
-        <v>386.9653606749796</v>
+        <v>386.9725488260881</v>
       </c>
       <c r="B320" t="n">
-        <v>-15.521495918124</v>
+        <v>-15.5220999931997</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="1" t="n">
-        <v>389.5554528331833</v>
+        <v>389.562887656147</v>
       </c>
       <c r="B321" t="n">
-        <v>-15.74047505754706</v>
+        <v>-15.74110531402619</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="1" t="n">
-        <v>392.1358021354193</v>
+        <v>392.14348168136</v>
       </c>
       <c r="B322" t="n">
-        <v>-15.96051449702213</v>
+        <v>-15.96117114647009</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="n">
-        <v>394.7063540947545</v>
+        <v>394.7142671881351</v>
       </c>
       <c r="B323" t="n">
-        <v>-16.18160176750058</v>
+        <v>-16.18228422299813</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="1" t="n">
-        <v>397.2670258638165</v>
+        <v>397.2751826772408</v>
       </c>
       <c r="B324" t="n">
-        <v>-16.40372190827605</v>
+        <v>-16.40443141978318</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="1" t="n">
-        <v>399.8177536362505</v>
+        <v>399.8261513001669</v>
       </c>
       <c r="B325" t="n">
-        <v>-16.62686152667536</v>
+        <v>-16.62759822354343</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="1" t="n">
-        <v>402.3584685722021</v>
+        <v>402.3671094265976</v>
       </c>
       <c r="B326" t="n">
-        <v>-16.85100673823592</v>
+        <v>-16.85177120736259</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="1" t="n">
-        <v>404.8890949892802</v>
+        <v>404.8979913215935</v>
       </c>
       <c r="B327" t="n">
-        <v>-17.07614298765287</v>
+        <v>-17.07693671246278</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="1" t="n">
-        <v>407.4095785715107</v>
+        <v>407.4187255287925</v>
       </c>
       <c r="B328" t="n">
-        <v>-17.30225756619771</v>
+        <v>-17.30308051645417</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="1" t="n">
-        <v>409.919845040956</v>
+        <v>409.9292280051077</v>
       </c>
       <c r="B329" t="n">
-        <v>-17.52933593975706</v>
+        <v>-17.53018719021645</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="1" t="n">
-        <v>412.419822252892</v>
+        <v>412.4294485844933</v>
       </c>
       <c r="B330" t="n">
-        <v>-17.75736369988815</v>
+        <v>-17.75824430810582</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="1" t="n">
-        <v>414.9094283812789</v>
+        <v>414.9193143651427</v>
       </c>
       <c r="B331" t="n">
-        <v>-17.98632548271763</v>
+        <v>-17.9872373496481</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="1" t="n">
-        <v>417.3886151257879</v>
+        <v>417.3987559370753</v>
       </c>
       <c r="B332" t="n">
-        <v>-18.21620895585957</v>
+        <v>-18.217152057975</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="1" t="n">
-        <v>419.8573004022459</v>
+        <v>419.8676877927811</v>
       </c>
       <c r="B333" t="n">
-        <v>-18.4469986322209</v>
+        <v>-18.44797261647108</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="1" t="n">
-        <v>422.3154161322108</v>
+        <v>422.3260546174901</v>
       </c>
       <c r="B334" t="n">
-        <v>-18.67868026445052</v>
+        <v>-18.67968597038731</v>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="1" t="n">
-        <v>424.7628986063081</v>
+        <v>424.773782497233</v>
       </c>
       <c r="B335" t="n">
-        <v>-18.91123998237774</v>
+        <v>-18.9122772899515</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="1" t="n">
-        <v>427.1996572789531</v>
+        <v>427.2108005390471</v>
       </c>
       <c r="B336" t="n">
-        <v>-19.14466131186043</v>
+        <v>-19.14573198114323</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="1" t="n">
-        <v>429.6256391806845</v>
+        <v>429.6370494468468</v>
       </c>
       <c r="B337" t="n">
-        <v>-19.37893131719929</v>
+        <v>-19.3800365316913</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="1" t="n">
-        <v>432.0407666402733</v>
+        <v>432.0524319246359</v>
       </c>
       <c r="B338" t="n">
-        <v>-19.6140346648705</v>
+        <v>-19.61517371173696</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="1" t="n">
-        <v>434.4449663148073</v>
+        <v>434.4568947466847</v>
       </c>
       <c r="B339" t="n">
-        <v>-19.84995639005726</v>
+        <v>-19.85113051437992</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="1" t="n">
-        <v>436.8381691514398</v>
+        <v>436.8503685072328</v>
       </c>
       <c r="B340" t="n">
-        <v>-20.08668191261995</v>
+        <v>-20.08789234811206</v>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="1" t="n">
-        <v>439.2203018709669</v>
+        <v>439.2327546081752</v>
       </c>
       <c r="B341" t="n">
-        <v>-20.32419620551451</v>
+        <v>-20.32544167432349</v>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="1" t="n">
-        <v>441.5913002893877</v>
+        <v>441.6040199226645</v>
       </c>
       <c r="B342" t="n">
-        <v>-20.56248512571966</v>
+        <v>-20.563767446848</v>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="1" t="n">
-        <v>443.9510809016919</v>
+        <v>443.9640628531031</v>
       </c>
       <c r="B343" t="n">
-        <v>-20.8015325650257</v>
+        <v>-20.80285175441722</v>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="1" t="n">
-        <v>446.2995692755619</v>
+        <v>446.3128150732211</v>
       </c>
       <c r="B344" t="n">
-        <v>-21.0413232871046</v>
+        <v>-21.04267998051483</v>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="1" t="n">
-        <v>448.6367001382736</v>
+        <v>448.6502083234316</v>
       </c>
       <c r="B345" t="n">
-        <v>-21.28184297672107</v>
+        <v>-21.28323751058895</v>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="1" t="n">
-        <v>450.9624048621395</v>
+        <v>450.9761801456556</v>
       </c>
       <c r="B346" t="n">
-        <v>-21.52307697903214</v>
+        <v>-21.52451033449461</v>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="1" t="n">
-        <v>453.2765919478367</v>
+        <v>453.2906459936422</v>
       </c>
       <c r="B347" t="n">
-        <v>-21.76500824360932</v>
+        <v>-21.76648214830672</v>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="1" t="n">
-        <v>455.5791954891408</v>
+        <v>455.5935294278781</v>
       </c>
       <c r="B348" t="n">
-        <v>-22.00762236082335</v>
+        <v>-22.009137463229</v>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="1" t="n">
-        <v>457.8701455325519</v>
+        <v>457.8847616684391</v>
       </c>
       <c r="B349" t="n">
-        <v>-22.2509045134876</v>
+        <v>-22.25246159673915</v>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="1" t="n">
-        <v>460.1493750065135</v>
+        <v>460.1642660975166</v>
       </c>
       <c r="B350" t="n">
-        <v>-22.4948402111157</v>
+        <v>-22.49643904533838</v>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="1" t="n">
-        <v>462.4167922057921</v>
+        <v>462.4319596811087</v>
       </c>
       <c r="B351" t="n">
-        <v>-22.73941232961241</v>
+        <v>-22.74105361230855</v>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="1" t="n">
-        <v>464.6723354806541</v>
+        <v>464.6877853317664</v>
       </c>
       <c r="B352" t="n">
-        <v>-22.98460698155566</v>
+        <v>-22.98629191932147</v>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="1" t="n">
-        <v>466.9159344974843</v>
+        <v>466.9316593901643</v>
       </c>
       <c r="B353" t="n">
-        <v>-23.23040939034865</v>
+        <v>-23.23213774742533</v>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="1" t="n">
-        <v>469.1474963314266</v>
+        <v>469.1635083959185</v>
       </c>
       <c r="B354" t="n">
-        <v>-23.47680232132336</v>
+        <v>-23.47857600789712</v>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="1" t="n">
-        <v>471.366963288048</v>
+        <v>471.3832617120587</v>
       </c>
       <c r="B355" t="n">
-        <v>-23.72377244926514</v>
+        <v>-23.72559197031023</v>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="1" t="n">
-        <v>473.5742486517984</v>
+        <v>473.5908491053529</v>
       </c>
       <c r="B356" t="n">
-        <v>-23.97130328919479</v>
+        <v>-23.97317101155505</v>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="1" t="n">
-        <v>475.7692884234614</v>
+        <v>475.7861775554152</v>
       </c>
       <c r="B357" t="n">
-        <v>-24.21938094740122</v>
+        <v>-24.22129599626894</v>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="1" t="n">
-        <v>477.9519993870979</v>
+        <v>477.969196724789</v>
       </c>
       <c r="B358" t="n">
-        <v>-24.46798943879043</v>
+        <v>-24.46995467320207</v>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="1" t="n">
-        <v>480.1223246090354</v>
+        <v>480.1398239906171</v>
       </c>
       <c r="B359" t="n">
-        <v>-24.71711585415602</v>
+        <v>-24.71913123610898</v>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="1" t="n">
-        <v>482.2801950662918</v>
+        <v>482.2979838085744</v>
       </c>
       <c r="B360" t="n">
-        <v>-24.96674603524787</v>
+        <v>-24.96881076414058</v>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="1" t="n">
-        <v>484.4255098496301</v>
+        <v>484.4436077164808</v>
       </c>
       <c r="B361" t="n">
-        <v>-25.21686221767368</v>
+        <v>-25.21897926681848</v>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="1" t="n">
-        <v>486.5582237704055</v>
+        <v>486.5766382787576</v>
       </c>
       <c r="B362" t="n">
-        <v>-25.46745323010077</v>
+        <v>-25.46962419573595</v>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="1" t="n">
-        <v>488.6782505794302</v>
+        <v>488.6969859144046</v>
       </c>
       <c r="B363" t="n">
-        <v>-25.71850326295043</v>
+        <v>-25.72072937845752</v>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="1" t="n">
-        <v>490.7855347812896</v>
+        <v>490.8045891470704</v>
       </c>
       <c r="B364" t="n">
-        <v>-25.97000029715102</v>
+        <v>-25.97228210576662</v>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="1" t="n">
-        <v>492.8800095788409</v>
+        <v>492.8993847100127</v>
       </c>
       <c r="B365" t="n">
-        <v>-26.22193118886997</v>
+        <v>-26.22426967017111</v>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="1" t="n">
-        <v>494.961606367523</v>
+        <v>494.9813209202326</v>
       </c>
       <c r="B366" t="n">
-        <v>-26.47428279183995</v>
+        <v>-26.47668100562902</v>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="1" t="n">
-        <v>497.0302626045175</v>
+        <v>497.0503225650972</v>
       </c>
       <c r="B367" t="n">
-        <v>-26.72704293500914</v>
+        <v>-26.72950245754055</v>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="1" t="n">
-        <v>499.0859352644209</v>
+        <v>499.1063266070253</v>
       </c>
       <c r="B368" t="n">
-        <v>-26.98020213862799</v>
+        <v>-26.9827221082495</v>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="1" t="n">
-        <v>501.128550796317</v>
+        <v>501.1492972948251</v>
       </c>
       <c r="B369" t="n">
-        <v>-27.23374750091972</v>
+        <v>-27.23633174473943</v>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="1" t="n">
-        <v>503.1580634223577</v>
+        <v>503.1791588015211</v>
       </c>
       <c r="B370" t="n">
-        <v>-27.48766989809937</v>
+        <v>-27.49031855995446</v>
       </c>
     </row>
     <row r="371">
       <c r="A371" s="1" t="n">
-        <v>505.1744147975543</v>
+        <v>505.1958805930281</v>
       </c>
       <c r="B371" t="n">
-        <v>-27.7419590465278</v>
+        <v>-27.74467579526438</v>
       </c>
     </row>
     <row r="372">
       <c r="A372" s="1" t="n">
-        <v>507.1775826033028</v>
+        <v>507.1994241214705</v>
       </c>
       <c r="B372" t="n">
-        <v>-27.996609674826</v>
+        <v>-27.99939619831866</v>
       </c>
     </row>
     <row r="373">
       <c r="A373" s="1" t="n">
-        <v>509.1675273085694</v>
+        <v>509.1897369028907</v>
       </c>
       <c r="B373" t="n">
-        <v>-28.25161489819328</v>
+        <v>-28.25447126028155</v>
       </c>
     </row>
     <row r="374">
       <c r="A374" s="1" t="n">
-        <v>511.1442133936517</v>
+        <v>511.166825332004</v>
       </c>
       <c r="B374" t="n">
-        <v>-28.50696892591463</v>
+        <v>-28.50990063175146</v>
       </c>
     </row>
     <row r="375">
       <c r="A375" s="1" t="n">
-        <v>513.1076383016425</v>
+        <v>513.1306502088964</v>
       </c>
       <c r="B375" t="n">
-        <v>-28.76267091426166</v>
+        <v>-28.76567881680103</v>
       </c>
     </row>
     <row r="376">
       <c r="A376" s="1" t="n">
-        <v>515.0577754858793</v>
+        <v>515.0812030706855</v>
       </c>
       <c r="B376" t="n">
-        <v>-29.01871768894986</v>
+        <v>-29.02180505102399</v>
       </c>
     </row>
     <row r="377">
       <c r="A377" s="1" t="n">
-        <v>516.9946418144401</v>
+        <v>517.0185057334626</v>
       </c>
       <c r="B377" t="n">
-        <v>-29.2751126340552</v>
+        <v>-29.27828346470437</v>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="1" t="n">
-        <v>518.9182618923427</v>
+        <v>518.9425738448315</v>
       </c>
       <c r="B378" t="n">
-        <v>-29.53186121543803</v>
+        <v>-29.53511843209753</v>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="1" t="n">
-        <v>520.8286672211713</v>
+        <v>520.8534295114689</v>
       </c>
       <c r="B379" t="n">
-        <v>-29.78897098893998</v>
+        <v>-29.79231632309848</v>
       </c>
     </row>
     <row r="380">
       <c r="A380" s="1" t="n">
-        <v>522.7259058166068</v>
+        <v>522.7511582788068</v>
       </c>
       <c r="B380" t="n">
-        <v>-30.04645303784031</v>
+        <v>-30.04989339295116</v>
       </c>
     </row>
     <row r="381">
       <c r="A381" s="1" t="n">
-        <v>524.6100786912355</v>
+        <v>524.6358312734219</v>
       </c>
       <c r="B381" t="n">
-        <v>-30.30432717970746</v>
+        <v>-30.30786554435505</v>
       </c>
     </row>
     <row r="382">
       <c r="A382" s="1" t="n">
-        <v>526.4812762673264</v>
+        <v>526.5075478920714</v>
       </c>
       <c r="B382" t="n">
-        <v>-30.56261357842527</v>
+        <v>-30.56625428074909</v>
       </c>
     </row>
   </sheetData>

</xml_diff>